<commit_message>
Version 04 | A single etf.py file for ETF and ice.py file for ICE
</commit_message>
<xml_diff>
--- a/Data/PFTF-Projected.xlsx
+++ b/Data/PFTF-Projected.xlsx
@@ -5,7 +5,7 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="PFTF0313 " sheetId="1" r:id="rId2"/>
+    <sheet name="PFTF0330 " sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
@@ -14,7 +14,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="273">
   <si>
-    <t xml:space="preserve">PFTF for 03/13/2023  ( Projected Universe )</t>
+    <t xml:space="preserve">PFTF for 03/30/2023  ( Projected Universe )</t>
   </si>
   <si>
     <t>Cusip</t>
@@ -1103,61 +1103,61 @@
         <v>46</v>
       </c>
       <c r="N3" s="0">
-        <v>454.241</v>
+        <v>441.3</v>
       </c>
       <c r="O3" s="0">
-        <v>82.6</v>
+        <v>89.49</v>
       </c>
       <c r="P3" s="0">
         <v>0</v>
       </c>
       <c r="Q3" s="0">
-        <v>1.45922</v>
+        <v>1.48106</v>
       </c>
       <c r="R3" s="0">
-        <v>1.41711</v>
+        <v>1.38153</v>
       </c>
       <c r="S3" s="0">
         <v>0</v>
       </c>
       <c r="T3" s="0">
-        <v>540</v>
+        <v>455</v>
       </c>
       <c r="U3" s="0">
-        <v>85</v>
+        <v>0</v>
       </c>
       <c r="V3" s="0">
-        <v>492</v>
+        <v>446</v>
       </c>
       <c r="W3" s="0">
-        <v>38</v>
+        <v>-8</v>
       </c>
       <c r="X3" s="0">
-        <v>9.29</v>
+        <v>8.51</v>
       </c>
       <c r="Y3" s="0">
-        <v>19.12</v>
+        <v>13.65</v>
       </c>
       <c r="Z3" s="0">
-        <v>19.12</v>
+        <v>13.65</v>
       </c>
       <c r="AA3" s="0">
-        <v>-7.524</v>
+        <v>0.188</v>
       </c>
       <c r="AB3" s="0">
-        <v>-7.962</v>
+        <v>0.189</v>
       </c>
       <c r="AC3" s="0">
-        <v>-0.01</v>
+        <v>0.66</v>
       </c>
       <c r="AD3" s="0">
-        <v>1.44</v>
+        <v>1.48</v>
       </c>
       <c r="AE3" s="0">
-        <v>1.44</v>
+        <v>1.48</v>
       </c>
       <c r="AF3" s="0">
-        <v>-0.31</v>
+        <v>-0.19</v>
       </c>
       <c r="AG3" s="0">
         <v>0.03</v>
@@ -1210,61 +1210,61 @@
         <v>46</v>
       </c>
       <c r="N4" s="0">
-        <v>340.68</v>
+        <v>330.975</v>
       </c>
       <c r="O4" s="0">
-        <v>94</v>
+        <v>96.08</v>
       </c>
       <c r="P4" s="0">
         <v>0</v>
       </c>
       <c r="Q4" s="0">
-        <v>1.24545</v>
+        <v>1.19262</v>
       </c>
       <c r="R4" s="0">
-        <v>1.15802</v>
+        <v>1.12895</v>
       </c>
       <c r="S4" s="0">
         <v>0</v>
       </c>
       <c r="T4" s="0">
-        <v>544</v>
+        <v>462</v>
       </c>
       <c r="U4" s="0">
-        <v>230</v>
+        <v>148</v>
       </c>
       <c r="V4" s="0">
-        <v>604</v>
+        <v>549</v>
       </c>
       <c r="W4" s="0">
-        <v>161</v>
+        <v>106</v>
       </c>
       <c r="X4" s="0">
-        <v>9.33</v>
+        <v>8.56</v>
       </c>
       <c r="Y4" s="0">
-        <v>9.81</v>
+        <v>8.79</v>
       </c>
       <c r="Z4" s="0">
-        <v>9.81</v>
+        <v>8.79</v>
       </c>
       <c r="AA4" s="0">
-        <v>-3.411</v>
+        <v>-1.274</v>
       </c>
       <c r="AB4" s="0">
-        <v>-5.012</v>
+        <v>-2.904</v>
       </c>
       <c r="AC4" s="0">
-        <v>2.04</v>
+        <v>2.12</v>
       </c>
       <c r="AD4" s="0">
-        <v>2.13</v>
+        <v>2.14</v>
       </c>
       <c r="AE4" s="0">
-        <v>2.13</v>
+        <v>2.14</v>
       </c>
       <c r="AF4" s="0">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="AG4" s="0">
         <v>0.06</v>
@@ -1317,58 +1317,58 @@
         <v>57</v>
       </c>
       <c r="N5" s="0">
-        <v>510.278</v>
+        <v>540.996</v>
       </c>
       <c r="O5" s="0">
-        <v>79</v>
+        <v>78.32</v>
       </c>
       <c r="P5" s="0">
         <v>0</v>
       </c>
       <c r="Q5" s="0">
-        <v>1.56779</v>
+        <v>1.58906</v>
       </c>
       <c r="R5" s="0">
-        <v>1.54203</v>
+        <v>1.64054</v>
       </c>
       <c r="S5" s="0">
         <v>0</v>
       </c>
       <c r="T5" s="0">
-        <v>586</v>
+        <v>565</v>
       </c>
       <c r="U5" s="0">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="V5" s="0">
-        <v>519</v>
+        <v>512</v>
       </c>
       <c r="W5" s="0">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="X5" s="0">
-        <v>11</v>
+        <v>11.32</v>
       </c>
       <c r="Y5" s="0">
-        <v>19.03</v>
+        <v>19.52</v>
       </c>
       <c r="Z5" s="0">
-        <v>19.03</v>
+        <v>19.52</v>
       </c>
       <c r="AA5" s="0">
-        <v>-8.692</v>
+        <v>-7.708</v>
       </c>
       <c r="AB5" s="0">
-        <v>-9.804</v>
+        <v>-8.932</v>
       </c>
       <c r="AC5" s="0">
-        <v>-0.35</v>
+        <v>-0.26</v>
       </c>
       <c r="AD5" s="0">
-        <v>1.76</v>
+        <v>1.75</v>
       </c>
       <c r="AE5" s="0">
-        <v>1.76</v>
+        <v>1.75</v>
       </c>
       <c r="AF5" s="0">
         <v>-0.43</v>
@@ -1424,52 +1424,52 @@
         <v>57</v>
       </c>
       <c r="N6" s="0">
-        <v>357.195</v>
+        <v>378.697</v>
       </c>
       <c r="O6" s="0">
-        <v>84.8</v>
+        <v>83.12</v>
       </c>
       <c r="P6" s="0">
         <v>0</v>
       </c>
       <c r="Q6" s="0">
-        <v>1.17802</v>
+        <v>1.18052</v>
       </c>
       <c r="R6" s="0">
-        <v>1.12134</v>
+        <v>1.19298</v>
       </c>
       <c r="S6" s="0">
         <v>0</v>
       </c>
       <c r="T6" s="0">
-        <v>553</v>
+        <v>545</v>
       </c>
       <c r="U6" s="0">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="V6" s="0">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="W6" s="0">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="X6" s="0">
-        <v>10.61</v>
+        <v>11.08</v>
       </c>
       <c r="Y6" s="0">
-        <v>18.22</v>
+        <v>19.71</v>
       </c>
       <c r="Z6" s="0">
-        <v>18.22</v>
+        <v>19.71</v>
       </c>
       <c r="AA6" s="0">
-        <v>-5.652</v>
+        <v>-5.713</v>
       </c>
       <c r="AB6" s="0">
-        <v>-6.465</v>
+        <v>-6.632</v>
       </c>
       <c r="AC6" s="0">
-        <v>-0.34</v>
+        <v>-0.33</v>
       </c>
       <c r="AD6" s="0">
         <v>1.35</v>
@@ -1531,61 +1531,61 @@
         <v>57</v>
       </c>
       <c r="N7" s="0">
-        <v>208.548</v>
+        <v>221.103</v>
       </c>
       <c r="O7" s="0">
-        <v>86</v>
+        <v>81.6</v>
       </c>
       <c r="P7" s="0">
         <v>0</v>
       </c>
       <c r="Q7" s="0">
-        <v>0.69752</v>
+        <v>0.67664</v>
       </c>
       <c r="R7" s="0">
-        <v>0.65994</v>
+        <v>0.7021</v>
       </c>
       <c r="S7" s="0">
         <v>0</v>
       </c>
       <c r="T7" s="0">
-        <v>479</v>
+        <v>510</v>
       </c>
       <c r="U7" s="0">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="V7" s="0">
-        <v>456</v>
+        <v>471</v>
       </c>
       <c r="W7" s="0">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="X7" s="0">
-        <v>9.89</v>
+        <v>10.89</v>
       </c>
       <c r="Y7" s="0">
-        <v>22.64</v>
+        <v>28.5</v>
       </c>
       <c r="Z7" s="0">
-        <v>22.64</v>
+        <v>28.5</v>
       </c>
       <c r="AA7" s="0">
-        <v>-5.077</v>
+        <v>-8.037</v>
       </c>
       <c r="AB7" s="0">
-        <v>-5.468</v>
+        <v>-8.574</v>
       </c>
       <c r="AC7" s="0">
-        <v>-1.04</v>
+        <v>-1.29</v>
       </c>
       <c r="AD7" s="0">
-        <v>0.91</v>
+        <v>0.89</v>
       </c>
       <c r="AE7" s="0">
-        <v>0.91</v>
+        <v>0.89</v>
       </c>
       <c r="AF7" s="0">
-        <v>-0.42</v>
+        <v>-0.46</v>
       </c>
       <c r="AG7" s="0">
         <v>0.01</v>
@@ -1638,19 +1638,19 @@
         <v>57</v>
       </c>
       <c r="N8" s="0">
-        <v>288.418</v>
+        <v>305.781</v>
       </c>
       <c r="O8" s="0">
-        <v>99.24</v>
+        <v>95.76</v>
       </c>
       <c r="P8" s="0">
         <v>0</v>
       </c>
       <c r="Q8" s="0">
-        <v>1.11317</v>
+        <v>1.09817</v>
       </c>
       <c r="R8" s="0">
-        <v>1.02631</v>
+        <v>1.09188</v>
       </c>
       <c r="S8" s="0">
         <v>0</v>
@@ -1677,10 +1677,10 @@
         <v>99.99</v>
       </c>
       <c r="AA8" s="0">
-        <v>-2.591</v>
+        <v>-3.568</v>
       </c>
       <c r="AB8" s="0">
-        <v>-2.449</v>
+        <v>-3.726</v>
       </c>
       <c r="AC8" s="0">
         <v>-1.09</v>
@@ -1742,52 +1742,52 @@
         <v>57</v>
       </c>
       <c r="N9" s="0">
-        <v>133.116</v>
+        <v>141.129</v>
       </c>
       <c r="O9" s="0">
-        <v>86</v>
+        <v>86.08</v>
       </c>
       <c r="P9" s="0">
         <v>0</v>
       </c>
       <c r="Q9" s="0">
-        <v>0.44523</v>
+        <v>0.45561</v>
       </c>
       <c r="R9" s="0">
-        <v>0.42533</v>
+        <v>0.4525</v>
       </c>
       <c r="S9" s="0">
         <v>0</v>
       </c>
       <c r="T9" s="0">
-        <v>505</v>
+        <v>475</v>
       </c>
       <c r="U9" s="0">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="V9" s="0">
-        <v>475</v>
+        <v>457</v>
       </c>
       <c r="W9" s="0">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="X9" s="0">
-        <v>8.72</v>
+        <v>8.6</v>
       </c>
       <c r="Y9" s="0">
-        <v>11.85</v>
+        <v>11.83</v>
       </c>
       <c r="Z9" s="0">
-        <v>11.85</v>
+        <v>11.83</v>
       </c>
       <c r="AA9" s="0">
-        <v>-5.99</v>
+        <v>-3.785</v>
       </c>
       <c r="AB9" s="0">
-        <v>-7.772</v>
+        <v>-5.572</v>
       </c>
       <c r="AC9" s="0">
-        <v>2.14</v>
+        <v>2.31</v>
       </c>
       <c r="AD9" s="0">
         <v>3.61</v>
@@ -1796,7 +1796,7 @@
         <v>3.61</v>
       </c>
       <c r="AF9" s="0">
-        <v>-0.21</v>
+        <v>-0.19</v>
       </c>
       <c r="AG9" s="0">
         <v>0.17</v>
@@ -1849,61 +1849,49 @@
         <v>71</v>
       </c>
       <c r="N10" s="0">
-        <v>567.801</v>
+        <v>551.625</v>
       </c>
       <c r="O10" s="0">
-        <v>100.72</v>
+        <v>101.36</v>
       </c>
       <c r="P10" s="0">
         <v>0</v>
       </c>
       <c r="Q10" s="0">
-        <v>2.22416</v>
+        <v>2.09693</v>
       </c>
       <c r="R10" s="0">
-        <v>2.01492</v>
+        <v>1.96433</v>
       </c>
       <c r="S10" s="0">
         <v>0</v>
       </c>
-      <c r="T10" s="0">
-        <v>191</v>
-      </c>
-      <c r="U10" s="0">
-        <v>710</v>
-      </c>
-      <c r="V10" s="0">
-        <v>248</v>
-      </c>
-      <c r="W10" s="0">
-        <v>1248</v>
-      </c>
       <c r="X10" s="0">
-        <v>7.18</v>
+        <v>-10</v>
       </c>
       <c r="Y10" s="0">
-        <v>-1.95</v>
+        <v>-9.2</v>
       </c>
       <c r="Z10" s="0">
-        <v>8.04</v>
+        <v>8.29</v>
       </c>
       <c r="AA10" s="0">
-        <v>-0.866</v>
+        <v>1.731</v>
       </c>
       <c r="AB10" s="0">
-        <v>-1.106</v>
+        <v>1.279</v>
       </c>
       <c r="AC10" s="0">
-        <v>-0.14</v>
+        <v>0.04</v>
       </c>
       <c r="AD10" s="0">
-        <v>0.04</v>
+        <v>0.09</v>
       </c>
       <c r="AE10" s="0">
-        <v>0.04</v>
+        <v>0.08</v>
       </c>
       <c r="AF10" s="0">
-        <v>-0.08</v>
+        <v>0</v>
       </c>
       <c r="AG10" s="0">
         <v>0</v>
@@ -1956,61 +1944,61 @@
         <v>80</v>
       </c>
       <c r="N11" s="0">
-        <v>397.46</v>
+        <v>386.137</v>
       </c>
       <c r="O11" s="0">
-        <v>93.68</v>
+        <v>93.04</v>
       </c>
       <c r="P11" s="0">
         <v>0</v>
       </c>
       <c r="Q11" s="0">
-        <v>1.44808</v>
+        <v>1.34737</v>
       </c>
       <c r="R11" s="0">
-        <v>1.28606</v>
+        <v>1.25377</v>
       </c>
       <c r="S11" s="0">
         <v>0</v>
       </c>
       <c r="T11" s="0">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="U11" s="0">
-        <v>-14</v>
+        <v>-13</v>
       </c>
       <c r="V11" s="0">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="W11" s="0">
-        <v>-6</v>
+        <v>-4</v>
       </c>
       <c r="X11" s="0">
-        <v>9.01</v>
+        <v>9.4</v>
       </c>
       <c r="Y11" s="0">
-        <v>11.88</v>
+        <v>12.48</v>
       </c>
       <c r="Z11" s="0">
-        <v>11.88</v>
+        <v>12.48</v>
       </c>
       <c r="AA11" s="0">
-        <v>1.123</v>
+        <v>2.105</v>
       </c>
       <c r="AB11" s="0">
-        <v>0.367</v>
+        <v>1.301</v>
       </c>
       <c r="AC11" s="0">
-        <v>0.94</v>
+        <v>0.9</v>
       </c>
       <c r="AD11" s="0">
-        <v>1.15</v>
+        <v>1.14</v>
       </c>
       <c r="AE11" s="0">
-        <v>1.15</v>
+        <v>1.14</v>
       </c>
       <c r="AF11" s="0">
-        <v>0.07</v>
+        <v>0.01</v>
       </c>
       <c r="AG11" s="0">
         <v>0.02</v>
@@ -2063,61 +2051,61 @@
         <v>71</v>
       </c>
       <c r="N12" s="0">
-        <v>170.34</v>
+        <v>165.487</v>
       </c>
       <c r="O12" s="0">
-        <v>93.23</v>
+        <v>90.24</v>
       </c>
       <c r="P12" s="0">
         <v>0</v>
       </c>
       <c r="Q12" s="0">
-        <v>0.61766</v>
+        <v>0.56006</v>
       </c>
       <c r="R12" s="0">
-        <v>0.57616</v>
+        <v>0.56169</v>
       </c>
       <c r="S12" s="0">
         <v>0</v>
       </c>
       <c r="T12" s="0">
-        <v>609</v>
+        <v>673</v>
       </c>
       <c r="U12" s="0">
-        <v>247</v>
+        <v>311</v>
       </c>
       <c r="V12" s="0">
-        <v>638</v>
+        <v>658</v>
       </c>
       <c r="W12" s="0">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="X12" s="0">
-        <v>9.8</v>
+        <v>10.46</v>
       </c>
       <c r="Y12" s="0">
-        <v>10.43</v>
+        <v>11.95</v>
       </c>
       <c r="Z12" s="0">
-        <v>10.43</v>
+        <v>11.95</v>
       </c>
       <c r="AA12" s="0">
-        <v>-3.723</v>
+        <v>-6.815</v>
       </c>
       <c r="AB12" s="0">
-        <v>-5.333</v>
+        <v>-8.455</v>
       </c>
       <c r="AC12" s="0">
-        <v>2.07</v>
+        <v>1.88</v>
       </c>
       <c r="AD12" s="0">
-        <v>2.15</v>
+        <v>2.13</v>
       </c>
       <c r="AE12" s="0">
-        <v>2.15</v>
+        <v>2.13</v>
       </c>
       <c r="AF12" s="0">
-        <v>0.04</v>
+        <v>-0</v>
       </c>
       <c r="AG12" s="0">
         <v>0.06</v>
@@ -2170,61 +2158,61 @@
         <v>46</v>
       </c>
       <c r="N13" s="0">
-        <v>765.417</v>
+        <v>774.832</v>
       </c>
       <c r="O13" s="0">
-        <v>86.12</v>
+        <v>88.12</v>
       </c>
       <c r="P13" s="0">
         <v>0</v>
       </c>
       <c r="Q13" s="0">
-        <v>2.56363</v>
+        <v>2.56069</v>
       </c>
       <c r="R13" s="0">
-        <v>2.64455</v>
+        <v>2.68639</v>
       </c>
       <c r="S13" s="0">
         <v>0</v>
       </c>
       <c r="T13" s="0">
+        <v>418</v>
+      </c>
+      <c r="U13" s="0">
+        <v>149</v>
+      </c>
+      <c r="V13" s="0">
         <v>440</v>
       </c>
-      <c r="U13" s="0">
-        <v>171</v>
-      </c>
-      <c r="V13" s="0">
-        <v>448</v>
-      </c>
       <c r="W13" s="0">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="X13" s="0">
-        <v>9.3</v>
+        <v>9.26</v>
       </c>
       <c r="Y13" s="0">
-        <v>9.42</v>
+        <v>8.95</v>
       </c>
       <c r="Z13" s="0">
-        <v>9.42</v>
+        <v>8.95</v>
       </c>
       <c r="AA13" s="0">
-        <v>-12.94</v>
+        <v>-9.313</v>
       </c>
       <c r="AB13" s="0">
-        <v>-15.438</v>
+        <v>-11.914</v>
       </c>
       <c r="AC13" s="0">
-        <v>4.16</v>
+        <v>4.33</v>
       </c>
       <c r="AD13" s="0">
-        <v>4.88</v>
+        <v>4.9</v>
       </c>
       <c r="AE13" s="0">
-        <v>4.88</v>
+        <v>4.9</v>
       </c>
       <c r="AF13" s="0">
-        <v>0.05</v>
+        <v>0.09</v>
       </c>
       <c r="AG13" s="0">
         <v>0.31</v>
@@ -2277,52 +2265,52 @@
         <v>46</v>
       </c>
       <c r="N14" s="0">
-        <v>532.464</v>
+        <v>539.013</v>
       </c>
       <c r="O14" s="0">
-        <v>90.72</v>
+        <v>91.6</v>
       </c>
       <c r="P14" s="0">
         <v>0</v>
       </c>
       <c r="Q14" s="0">
-        <v>1.87865</v>
+        <v>1.85169</v>
       </c>
       <c r="R14" s="0">
-        <v>1.87539</v>
+        <v>1.90506</v>
       </c>
       <c r="S14" s="0">
         <v>0</v>
       </c>
       <c r="T14" s="0">
-        <v>577</v>
+        <v>559</v>
       </c>
       <c r="U14" s="0">
-        <v>403</v>
+        <v>385</v>
       </c>
       <c r="V14" s="0">
-        <v>600</v>
+        <v>582</v>
       </c>
       <c r="W14" s="0">
-        <v>313</v>
+        <v>295</v>
       </c>
       <c r="X14" s="0">
-        <v>9.75</v>
+        <v>9.64</v>
       </c>
       <c r="Y14" s="0">
-        <v>10.81</v>
+        <v>10.37</v>
       </c>
       <c r="Z14" s="0">
-        <v>10.81</v>
+        <v>10.37</v>
       </c>
       <c r="AA14" s="0">
-        <v>-10.036</v>
+        <v>-7.583</v>
       </c>
       <c r="AB14" s="0">
-        <v>-11.617</v>
+        <v>-9.193</v>
       </c>
       <c r="AC14" s="0">
-        <v>2</v>
+        <v>2.06</v>
       </c>
       <c r="AD14" s="0">
         <v>2.2</v>
@@ -2331,7 +2319,7 @@
         <v>2.2</v>
       </c>
       <c r="AF14" s="0">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="AG14" s="0">
         <v>0.07</v>
@@ -2384,52 +2372,52 @@
         <v>46</v>
       </c>
       <c r="N15" s="0">
-        <v>443.72</v>
+        <v>449.178</v>
       </c>
       <c r="O15" s="0">
-        <v>93.08</v>
+        <v>92.88</v>
       </c>
       <c r="P15" s="0">
         <v>0</v>
       </c>
       <c r="Q15" s="0">
-        <v>1.60627</v>
+        <v>1.56464</v>
       </c>
       <c r="R15" s="0">
-        <v>1.61366</v>
+        <v>1.63919</v>
       </c>
       <c r="S15" s="0">
         <v>0</v>
       </c>
       <c r="T15" s="0">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="U15" s="0">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="V15" s="0">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="W15" s="0">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="X15" s="0">
-        <v>8.24</v>
+        <v>8.27</v>
       </c>
       <c r="Y15" s="0">
-        <v>9.7</v>
+        <v>9.76</v>
       </c>
       <c r="Z15" s="0">
-        <v>9.7</v>
+        <v>9.76</v>
       </c>
       <c r="AA15" s="0">
-        <v>-10.603</v>
+        <v>-8.562</v>
       </c>
       <c r="AB15" s="0">
-        <v>-12.235</v>
+        <v>-10.295</v>
       </c>
       <c r="AC15" s="0">
-        <v>3.19</v>
+        <v>3.18</v>
       </c>
       <c r="AD15" s="0">
         <v>3.8</v>
@@ -2438,7 +2426,7 @@
         <v>3.8</v>
       </c>
       <c r="AF15" s="0">
-        <v>-0.01</v>
+        <v>-0.02</v>
       </c>
       <c r="AG15" s="0">
         <v>0.19</v>
@@ -2491,52 +2479,52 @@
         <v>97</v>
       </c>
       <c r="N16" s="0">
-        <v>278.004</v>
+        <v>281.423</v>
       </c>
       <c r="O16" s="0">
-        <v>81.52</v>
+        <v>83.64</v>
       </c>
       <c r="P16" s="0">
         <v>0</v>
       </c>
       <c r="Q16" s="0">
-        <v>0.88139</v>
+        <v>0.88277</v>
       </c>
       <c r="R16" s="0">
-        <v>0.8137</v>
+        <v>0.82657</v>
       </c>
       <c r="S16" s="0">
         <v>0</v>
       </c>
       <c r="T16" s="0">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="U16" s="0">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="V16" s="0">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="W16" s="0">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="X16" s="0">
-        <v>6.05</v>
+        <v>6.18</v>
       </c>
       <c r="Y16" s="0">
-        <v>6.48</v>
+        <v>6.68</v>
       </c>
       <c r="Z16" s="0">
-        <v>6.48</v>
+        <v>6.68</v>
       </c>
       <c r="AA16" s="0">
-        <v>-2.721</v>
+        <v>-0.191</v>
       </c>
       <c r="AB16" s="0">
-        <v>-3.688</v>
+        <v>-1.022</v>
       </c>
       <c r="AC16" s="0">
-        <v>5.11</v>
+        <v>4.88</v>
       </c>
       <c r="AD16" s="0">
         <v>0.08</v>
@@ -2545,7 +2533,7 @@
         <v>0.08</v>
       </c>
       <c r="AF16" s="0">
-        <v>34.1</v>
+        <v>31.77</v>
       </c>
       <c r="AG16" s="0">
         <v>0</v>
@@ -2598,52 +2586,52 @@
         <v>97</v>
       </c>
       <c r="N17" s="0">
-        <v>370.663</v>
+        <v>375.223</v>
       </c>
       <c r="O17" s="0">
-        <v>79.8</v>
+        <v>81</v>
       </c>
       <c r="P17" s="0">
         <v>0</v>
       </c>
       <c r="Q17" s="0">
-        <v>1.15036</v>
+        <v>1.13985</v>
       </c>
       <c r="R17" s="0">
-        <v>1.08128</v>
+        <v>1.09839</v>
       </c>
       <c r="S17" s="0">
         <v>0</v>
       </c>
       <c r="T17" s="0">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="U17" s="0">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="V17" s="0">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="W17" s="0">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="X17" s="0">
-        <v>6.42</v>
+        <v>6.67</v>
       </c>
       <c r="Y17" s="0">
-        <v>6.81</v>
+        <v>7.09</v>
       </c>
       <c r="Z17" s="0">
-        <v>6.81</v>
+        <v>7.09</v>
       </c>
       <c r="AA17" s="0">
-        <v>-4.454</v>
+        <v>-3.017</v>
       </c>
       <c r="AB17" s="0">
-        <v>-5.272</v>
+        <v>-3.743</v>
       </c>
       <c r="AC17" s="0">
-        <v>4.95</v>
+        <v>4.85</v>
       </c>
       <c r="AD17" s="0">
         <v>0.09</v>
@@ -2652,7 +2640,7 @@
         <v>0.09</v>
       </c>
       <c r="AF17" s="0">
-        <v>34.57</v>
+        <v>33.39</v>
       </c>
       <c r="AG17" s="0">
         <v>0</v>
@@ -2705,61 +2693,61 @@
         <v>97</v>
       </c>
       <c r="N18" s="0">
-        <v>186.629</v>
+        <v>188.924</v>
       </c>
       <c r="O18" s="0">
-        <v>81.8</v>
+        <v>83.6</v>
       </c>
       <c r="P18" s="0">
         <v>0</v>
       </c>
       <c r="Q18" s="0">
-        <v>0.59373</v>
+        <v>0.59234</v>
       </c>
       <c r="R18" s="0">
-        <v>0.54495</v>
+        <v>0.55357</v>
       </c>
       <c r="S18" s="0">
         <v>0</v>
       </c>
       <c r="T18" s="0">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="U18" s="0">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="V18" s="0">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="W18" s="0">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="X18" s="0">
-        <v>6.49</v>
+        <v>6.65</v>
       </c>
       <c r="Y18" s="0">
-        <v>6.95</v>
+        <v>7.17</v>
       </c>
       <c r="Z18" s="0">
-        <v>6.95</v>
+        <v>7.17</v>
       </c>
       <c r="AA18" s="0">
-        <v>-2.153</v>
+        <v>0</v>
       </c>
       <c r="AB18" s="0">
-        <v>-3.015</v>
+        <v>-0.819</v>
       </c>
       <c r="AC18" s="0">
-        <v>4.72</v>
+        <v>4.73</v>
       </c>
       <c r="AD18" s="0">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="AE18" s="0">
-        <v>0.11</v>
+        <v>0.12</v>
       </c>
       <c r="AF18" s="0">
-        <v>32.2</v>
+        <v>31.1</v>
       </c>
       <c r="AG18" s="0">
         <v>0</v>
@@ -2812,61 +2800,61 @@
         <v>97</v>
       </c>
       <c r="N19" s="0">
-        <v>265.354</v>
+        <v>268.617</v>
       </c>
       <c r="O19" s="0">
-        <v>78.04</v>
+        <v>83.08</v>
       </c>
       <c r="P19" s="0">
         <v>0</v>
       </c>
       <c r="Q19" s="0">
-        <v>0.80537</v>
+        <v>0.83696</v>
       </c>
       <c r="R19" s="0">
-        <v>0.76963</v>
+        <v>0.7818</v>
       </c>
       <c r="S19" s="0">
         <v>0</v>
       </c>
       <c r="T19" s="0">
-        <v>115</v>
+        <v>71</v>
       </c>
       <c r="U19" s="0">
-        <v>37</v>
+        <v>-7</v>
       </c>
       <c r="V19" s="0">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="W19" s="0">
-        <v>27</v>
+        <v>-2</v>
       </c>
       <c r="X19" s="0">
-        <v>6.74</v>
+        <v>6.5</v>
       </c>
       <c r="Y19" s="0">
-        <v>7.14</v>
+        <v>7.07</v>
       </c>
       <c r="Z19" s="0">
-        <v>7.14</v>
+        <v>7.07</v>
       </c>
       <c r="AA19" s="0">
-        <v>-6.021</v>
+        <v>0.048</v>
       </c>
       <c r="AB19" s="0">
-        <v>-6.115</v>
+        <v>-0.248</v>
       </c>
       <c r="AC19" s="0">
-        <v>-3.42</v>
+        <v>-2.66</v>
       </c>
       <c r="AD19" s="0">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="AE19" s="0">
-        <v>0.1</v>
+        <v>0.12</v>
       </c>
       <c r="AF19" s="0">
-        <v>3.52</v>
+        <v>2.79</v>
       </c>
       <c r="AG19" s="0">
         <v>0</v>
@@ -2919,67 +2907,67 @@
         <v>97</v>
       </c>
       <c r="N20" s="0">
-        <v>931.812</v>
+        <v>943.274</v>
       </c>
       <c r="O20" s="0">
-        <v>98.76</v>
+        <v>100.36</v>
       </c>
       <c r="P20" s="0">
         <v>0</v>
       </c>
       <c r="Q20" s="0">
-        <v>3.57901</v>
+        <v>3.55036</v>
       </c>
       <c r="R20" s="0">
-        <v>3.31709</v>
+        <v>3.36957</v>
       </c>
       <c r="S20" s="0">
         <v>0</v>
       </c>
       <c r="T20" s="0">
-        <v>-8</v>
+        <v>-133</v>
       </c>
       <c r="U20" s="0">
-        <v>209</v>
+        <v>84</v>
       </c>
       <c r="V20" s="0">
-        <v>39</v>
+        <v>-80</v>
       </c>
       <c r="W20" s="0">
-        <v>151</v>
+        <v>32</v>
       </c>
       <c r="X20" s="0">
-        <v>3.53</v>
+        <v>2.33</v>
       </c>
       <c r="Y20" s="0">
-        <v>6.61</v>
+        <v>2.18</v>
       </c>
       <c r="Z20" s="0">
-        <v>6.61</v>
+        <v>6.5</v>
       </c>
       <c r="AA20" s="0">
-        <v>-1.518</v>
+        <v>0.052</v>
       </c>
       <c r="AB20" s="0">
-        <v>-1.845</v>
+        <v>-0.469</v>
       </c>
       <c r="AC20" s="0">
-        <v>2.85</v>
+        <v>0.76</v>
       </c>
       <c r="AD20" s="0">
-        <v>14.12</v>
+        <v>0.08</v>
       </c>
       <c r="AE20" s="0">
-        <v>14.12</v>
+        <v>14.29</v>
       </c>
       <c r="AF20" s="0">
-        <v>-2.37</v>
+        <v>-1.46</v>
       </c>
       <c r="AG20" s="0">
-        <v>3.57</v>
+        <v>0</v>
       </c>
       <c r="AH20" s="0">
-        <v>3.57</v>
+        <v>3.65</v>
       </c>
       <c r="AI20" s="0" t="s">
         <v>107</v>
@@ -3026,67 +3014,67 @@
         <v>97</v>
       </c>
       <c r="N21" s="0">
-        <v>340.68</v>
+        <v>330.975</v>
       </c>
       <c r="O21" s="0">
-        <v>79.2</v>
+        <v>94.32</v>
       </c>
       <c r="P21" s="0">
         <v>0</v>
       </c>
       <c r="Q21" s="0">
-        <v>1.04936</v>
+        <v>1.17077</v>
       </c>
       <c r="R21" s="0">
-        <v>1.20895</v>
+        <v>1.1786</v>
       </c>
       <c r="S21" s="0">
         <v>0</v>
       </c>
       <c r="T21" s="0">
-        <v>506</v>
+        <v>322</v>
       </c>
       <c r="U21" s="0">
-        <v>446</v>
+        <v>262</v>
       </c>
       <c r="V21" s="0">
-        <v>439</v>
+        <v>362</v>
       </c>
       <c r="W21" s="0">
-        <v>393</v>
+        <v>316</v>
       </c>
       <c r="X21" s="0">
-        <v>10.65</v>
+        <v>8.96</v>
       </c>
       <c r="Y21" s="0">
-        <v>32.12</v>
+        <v>12.49</v>
       </c>
       <c r="Z21" s="0">
-        <v>32.12</v>
+        <v>12.49</v>
       </c>
       <c r="AA21" s="0">
-        <v>-22.047</v>
+        <v>-5.603</v>
       </c>
       <c r="AB21" s="0">
-        <v>-22.81</v>
+        <v>-6.436</v>
       </c>
       <c r="AC21" s="0">
-        <v>-1.87</v>
+        <v>0.15</v>
       </c>
       <c r="AD21" s="0">
-        <v>0.85</v>
+        <v>0.93</v>
       </c>
       <c r="AE21" s="0">
-        <v>0.85</v>
+        <v>0.93</v>
       </c>
       <c r="AF21" s="0">
-        <v>-0.62</v>
+        <v>-0.21</v>
       </c>
       <c r="AG21" s="0">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="AH21" s="0">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="AI21" s="0" t="s">
         <v>47</v>
@@ -3133,52 +3121,52 @@
         <v>117</v>
       </c>
       <c r="N22" s="0">
-        <v>559.284</v>
+        <v>543.351</v>
       </c>
       <c r="O22" s="0">
-        <v>99.32</v>
+        <v>98.16</v>
       </c>
       <c r="P22" s="0">
         <v>0</v>
       </c>
       <c r="Q22" s="0">
-        <v>2.16034</v>
+        <v>2.00027</v>
       </c>
       <c r="R22" s="0">
-        <v>2.00814</v>
+        <v>1.95772</v>
       </c>
       <c r="S22" s="0">
         <v>0</v>
       </c>
       <c r="T22" s="0">
-        <v>175</v>
+        <v>201</v>
       </c>
       <c r="U22" s="0">
-        <v>153</v>
+        <v>179</v>
       </c>
       <c r="V22" s="0">
-        <v>217</v>
+        <v>243</v>
       </c>
       <c r="W22" s="0">
-        <v>365</v>
+        <v>391</v>
       </c>
       <c r="X22" s="0">
-        <v>6.09</v>
+        <v>6.72</v>
       </c>
       <c r="Y22" s="0">
-        <v>7.31</v>
+        <v>8.16</v>
       </c>
       <c r="Z22" s="0">
-        <v>7.31</v>
+        <v>8.16</v>
       </c>
       <c r="AA22" s="0">
-        <v>-3.385</v>
+        <v>-2.872</v>
       </c>
       <c r="AB22" s="0">
-        <v>-4.456</v>
+        <v>-3.993</v>
       </c>
       <c r="AC22" s="0">
-        <v>1.02</v>
+        <v>0.88</v>
       </c>
       <c r="AD22" s="0">
         <v>1.38</v>
@@ -3187,7 +3175,7 @@
         <v>1.38</v>
       </c>
       <c r="AF22" s="0">
-        <v>-0.1</v>
+        <v>-0.11</v>
       </c>
       <c r="AG22" s="0">
         <v>0.03</v>
@@ -3240,61 +3228,61 @@
         <v>117</v>
       </c>
       <c r="N23" s="0">
-        <v>476.953</v>
+        <v>463.365</v>
       </c>
       <c r="O23" s="0">
-        <v>100.4</v>
+        <v>98.36</v>
       </c>
       <c r="P23" s="0">
         <v>0</v>
       </c>
       <c r="Q23" s="0">
-        <v>1.86236</v>
+        <v>1.70929</v>
       </c>
       <c r="R23" s="0">
-        <v>1.71253</v>
+        <v>1.66953</v>
       </c>
       <c r="S23" s="0">
         <v>0</v>
       </c>
       <c r="T23" s="0">
-        <v>144</v>
+        <v>224</v>
       </c>
       <c r="U23" s="0">
-        <v>149</v>
+        <v>229</v>
       </c>
       <c r="V23" s="0">
-        <v>174</v>
+        <v>272</v>
       </c>
       <c r="W23" s="0">
-        <v>403</v>
+        <v>501</v>
       </c>
       <c r="X23" s="0">
-        <v>5.7</v>
+        <v>7.03</v>
       </c>
       <c r="Y23" s="0">
-        <v>6.76</v>
+        <v>8.96</v>
       </c>
       <c r="Z23" s="0">
-        <v>6.76</v>
+        <v>8.96</v>
       </c>
       <c r="AA23" s="0">
-        <v>-2.335</v>
+        <v>-2.592</v>
       </c>
       <c r="AB23" s="0">
-        <v>-3.079</v>
+        <v>-3.412</v>
       </c>
       <c r="AC23" s="0">
-        <v>0.79</v>
+        <v>0.48</v>
       </c>
       <c r="AD23" s="0">
-        <v>0.94</v>
+        <v>0.93</v>
       </c>
       <c r="AE23" s="0">
-        <v>0.94</v>
+        <v>0.93</v>
       </c>
       <c r="AF23" s="0">
-        <v>-0.03</v>
+        <v>-0.12</v>
       </c>
       <c r="AG23" s="0">
         <v>0.02</v>
@@ -3347,61 +3335,61 @@
         <v>57</v>
       </c>
       <c r="N24" s="0">
-        <v>295.256</v>
+        <v>286.845</v>
       </c>
       <c r="O24" s="0">
-        <v>74.2</v>
+        <v>72.64</v>
       </c>
       <c r="P24" s="0">
         <v>0</v>
       </c>
       <c r="Q24" s="0">
-        <v>0.85203</v>
+        <v>0.78144</v>
       </c>
       <c r="R24" s="0">
-        <v>0.82666</v>
+        <v>0.8059</v>
       </c>
       <c r="S24" s="0">
         <v>0</v>
       </c>
       <c r="T24" s="0">
-        <v>694</v>
+        <v>713</v>
       </c>
       <c r="U24" s="0">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="V24" s="0">
-        <v>556</v>
+        <v>562</v>
       </c>
       <c r="W24" s="0">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="X24" s="0">
-        <v>12.25</v>
+        <v>12.85</v>
       </c>
       <c r="Y24" s="0">
-        <v>21.93</v>
+        <v>22.98</v>
       </c>
       <c r="Z24" s="0">
-        <v>21.93</v>
+        <v>22.98</v>
       </c>
       <c r="AA24" s="0">
-        <v>-7.435</v>
+        <v>-9.381</v>
       </c>
       <c r="AB24" s="0">
-        <v>-8.576</v>
+        <v>-10.647</v>
       </c>
       <c r="AC24" s="0">
-        <v>-0.36</v>
+        <v>-0.47</v>
       </c>
       <c r="AD24" s="0">
-        <v>2.03</v>
+        <v>2.02</v>
       </c>
       <c r="AE24" s="0">
-        <v>2.03</v>
+        <v>2.02</v>
       </c>
       <c r="AF24" s="0">
-        <v>-0.47</v>
+        <v>-0.48</v>
       </c>
       <c r="AG24" s="0">
         <v>0.06</v>
@@ -3454,52 +3442,52 @@
         <v>128</v>
       </c>
       <c r="N25" s="0">
-        <v>454.241</v>
+        <v>441.3</v>
       </c>
       <c r="O25" s="0">
-        <v>88.24</v>
+        <v>87.88</v>
       </c>
       <c r="P25" s="0">
         <v>0</v>
       </c>
       <c r="Q25" s="0">
-        <v>1.55885</v>
+        <v>1.45445</v>
       </c>
       <c r="R25" s="0">
-        <v>1.49517</v>
+        <v>1.45763</v>
       </c>
       <c r="S25" s="0">
         <v>0</v>
       </c>
       <c r="T25" s="0">
+        <v>437</v>
+      </c>
+      <c r="U25" s="0">
+        <v>94</v>
+      </c>
+      <c r="V25" s="0">
         <v>436</v>
       </c>
-      <c r="U25" s="0">
-        <v>93</v>
-      </c>
-      <c r="V25" s="0">
-        <v>435</v>
-      </c>
       <c r="W25" s="0">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X25" s="0">
-        <v>9.29</v>
+        <v>9.53</v>
       </c>
       <c r="Y25" s="0">
-        <v>10.1</v>
+        <v>10.2</v>
       </c>
       <c r="Z25" s="0">
-        <v>10.1</v>
+        <v>10.2</v>
       </c>
       <c r="AA25" s="0">
-        <v>-6.367</v>
+        <v>-6.749</v>
       </c>
       <c r="AB25" s="0">
-        <v>-8.561</v>
+        <v>-9.096</v>
       </c>
       <c r="AC25" s="0">
-        <v>3.24</v>
+        <v>3.21</v>
       </c>
       <c r="AD25" s="0">
         <v>4.24</v>
@@ -3508,7 +3496,7 @@
         <v>4.24</v>
       </c>
       <c r="AF25" s="0">
-        <v>-0.1</v>
+        <v>-0.11</v>
       </c>
       <c r="AG25" s="0">
         <v>0.23</v>
@@ -3561,61 +3549,61 @@
         <v>134</v>
       </c>
       <c r="N26" s="0">
-        <v>908.481</v>
+        <v>882.6</v>
       </c>
       <c r="O26" s="0">
-        <v>92.72</v>
+        <v>93.6</v>
       </c>
       <c r="P26" s="0">
         <v>0</v>
       </c>
       <c r="Q26" s="0">
-        <v>3.27599</v>
+        <v>3.09823</v>
       </c>
       <c r="R26" s="0">
-        <v>3.08807</v>
+        <v>3.01053</v>
       </c>
       <c r="S26" s="0">
         <v>0</v>
       </c>
       <c r="T26" s="0">
+        <v>511</v>
+      </c>
+      <c r="U26" s="0">
+        <v>71</v>
+      </c>
+      <c r="V26" s="0">
         <v>529</v>
       </c>
-      <c r="U26" s="0">
-        <v>89</v>
-      </c>
-      <c r="V26" s="0">
-        <v>535</v>
-      </c>
       <c r="W26" s="0">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="X26" s="0">
-        <v>10.62</v>
+        <v>10.78</v>
       </c>
       <c r="Y26" s="0">
-        <v>16.07</v>
+        <v>15.12</v>
       </c>
       <c r="Z26" s="0">
-        <v>16.07</v>
+        <v>15.12</v>
       </c>
       <c r="AA26" s="0">
-        <v>-4.727</v>
+        <v>-3.822</v>
       </c>
       <c r="AB26" s="0">
-        <v>-5.47</v>
+        <v>-4.641</v>
       </c>
       <c r="AC26" s="0">
-        <v>0.12</v>
+        <v>0.24</v>
       </c>
       <c r="AD26" s="0">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="AE26" s="0">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="AF26" s="0">
-        <v>-0.19</v>
+        <v>-0.18</v>
       </c>
       <c r="AG26" s="0">
         <v>0.02</v>
@@ -3668,61 +3656,61 @@
         <v>141</v>
       </c>
       <c r="N27" s="0">
-        <v>118.67</v>
+        <v>115.29</v>
       </c>
       <c r="O27" s="0">
-        <v>86.88</v>
+        <v>90.72</v>
       </c>
       <c r="P27" s="0">
         <v>0</v>
       </c>
       <c r="Q27" s="0">
-        <v>0.40097</v>
+        <v>0.39226</v>
       </c>
       <c r="R27" s="0">
-        <v>0.40023</v>
+        <v>0.39018</v>
       </c>
       <c r="S27" s="0">
         <v>0</v>
       </c>
       <c r="T27" s="0">
-        <v>766</v>
+        <v>697</v>
       </c>
       <c r="U27" s="0">
-        <v>169</v>
+        <v>100</v>
       </c>
       <c r="V27" s="0">
-        <v>720</v>
+        <v>699</v>
       </c>
       <c r="W27" s="0">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="X27" s="0">
-        <v>13</v>
+        <v>12.59</v>
       </c>
       <c r="Y27" s="0">
-        <v>19.53</v>
+        <v>16.11</v>
       </c>
       <c r="Z27" s="0">
-        <v>19.53</v>
+        <v>16.11</v>
       </c>
       <c r="AA27" s="0">
-        <v>-7.889</v>
+        <v>-3.912</v>
       </c>
       <c r="AB27" s="0">
-        <v>-8.823</v>
+        <v>-4.912</v>
       </c>
       <c r="AC27" s="0">
-        <v>0.24</v>
+        <v>0.55</v>
       </c>
       <c r="AD27" s="0">
-        <v>1.25</v>
+        <v>1.27</v>
       </c>
       <c r="AE27" s="0">
-        <v>1.25</v>
+        <v>1.27</v>
       </c>
       <c r="AF27" s="0">
-        <v>-0.19</v>
+        <v>-0.14</v>
       </c>
       <c r="AG27" s="0">
         <v>0.03</v>
@@ -3775,52 +3763,52 @@
         <v>146</v>
       </c>
       <c r="N28" s="0">
-        <v>665.567</v>
+        <v>673.753</v>
       </c>
       <c r="O28" s="0">
-        <v>78.44</v>
+        <v>80.44</v>
       </c>
       <c r="P28" s="0">
         <v>0</v>
       </c>
       <c r="Q28" s="0">
-        <v>2.0304</v>
+        <v>2.03258</v>
       </c>
       <c r="R28" s="0">
-        <v>1.95272</v>
+        <v>1.98361</v>
       </c>
       <c r="S28" s="0">
         <v>0</v>
       </c>
       <c r="T28" s="0">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="U28" s="0">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="V28" s="0">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="W28" s="0">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="X28" s="0">
-        <v>6.04</v>
+        <v>6.11</v>
       </c>
       <c r="Y28" s="0">
-        <v>7.25</v>
+        <v>7.45</v>
       </c>
       <c r="Z28" s="0">
-        <v>7.25</v>
+        <v>7.45</v>
       </c>
       <c r="AA28" s="0">
-        <v>-6.619</v>
+        <v>-4.238</v>
       </c>
       <c r="AB28" s="0">
-        <v>-7.244</v>
+        <v>-4.988</v>
       </c>
       <c r="AC28" s="0">
-        <v>1.77</v>
+        <v>2.02</v>
       </c>
       <c r="AD28" s="0">
         <v>0.06</v>
@@ -3829,7 +3817,7 @@
         <v>0.06</v>
       </c>
       <c r="AF28" s="0">
-        <v>24.42</v>
+        <v>24.05</v>
       </c>
       <c r="AG28" s="0">
         <v>0</v>
@@ -3882,61 +3870,61 @@
         <v>146</v>
       </c>
       <c r="N29" s="0">
-        <v>1198.022</v>
+        <v>1212.758</v>
       </c>
       <c r="O29" s="0">
-        <v>79</v>
+        <v>81.28</v>
       </c>
       <c r="P29" s="0">
         <v>0</v>
       </c>
       <c r="Q29" s="0">
-        <v>3.68082</v>
+        <v>3.69685</v>
       </c>
       <c r="R29" s="0">
-        <v>3.46636</v>
+        <v>3.52121</v>
       </c>
       <c r="S29" s="0">
         <v>0</v>
       </c>
       <c r="T29" s="0">
-        <v>129</v>
+        <v>105</v>
       </c>
       <c r="U29" s="0">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="V29" s="0">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="W29" s="0">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="X29" s="0">
-        <v>5.92</v>
+        <v>5.95</v>
       </c>
       <c r="Y29" s="0">
-        <v>7.1</v>
+        <v>7.28</v>
       </c>
       <c r="Z29" s="0">
-        <v>7.1</v>
+        <v>7.28</v>
       </c>
       <c r="AA29" s="0">
-        <v>-4.635</v>
+        <v>-1.883</v>
       </c>
       <c r="AB29" s="0">
-        <v>-5.208</v>
+        <v>-2.529</v>
       </c>
       <c r="AC29" s="0">
-        <v>3.3</v>
+        <v>3.31</v>
       </c>
       <c r="AD29" s="0">
-        <v>0.06</v>
+        <v>0.07</v>
       </c>
       <c r="AE29" s="0">
-        <v>0.06</v>
+        <v>0.07</v>
       </c>
       <c r="AF29" s="0">
-        <v>29.63</v>
+        <v>28.17</v>
       </c>
       <c r="AG29" s="0">
         <v>0</v>
@@ -3989,61 +3977,61 @@
         <v>146</v>
       </c>
       <c r="N30" s="0">
-        <v>621.208</v>
+        <v>628.849</v>
       </c>
       <c r="O30" s="0">
-        <v>98.84</v>
+        <v>100.84</v>
       </c>
       <c r="P30" s="0">
         <v>0</v>
       </c>
       <c r="Q30" s="0">
-        <v>2.38794</v>
+        <v>2.37823</v>
       </c>
       <c r="R30" s="0">
-        <v>2.1975</v>
+        <v>2.23227</v>
       </c>
       <c r="S30" s="0">
         <v>0</v>
       </c>
       <c r="T30" s="0">
-        <v>270</v>
+        <v>185</v>
       </c>
       <c r="U30" s="0">
-        <v>222</v>
+        <v>137</v>
       </c>
       <c r="V30" s="0">
-        <v>325</v>
+        <v>217</v>
       </c>
       <c r="W30" s="0">
-        <v>304</v>
+        <v>196</v>
       </c>
       <c r="X30" s="0">
-        <v>7.89</v>
+        <v>7.16</v>
       </c>
       <c r="Y30" s="0">
-        <v>8.43</v>
+        <v>6.48</v>
       </c>
       <c r="Z30" s="0">
-        <v>8.43</v>
+        <v>6.48</v>
       </c>
       <c r="AA30" s="0">
-        <v>-2.409</v>
+        <v>-0.434</v>
       </c>
       <c r="AB30" s="0">
-        <v>-3.238</v>
+        <v>-1.326</v>
       </c>
       <c r="AC30" s="0">
-        <v>0.68</v>
+        <v>1.02</v>
       </c>
       <c r="AD30" s="0">
-        <v>1.02</v>
+        <v>1.03</v>
       </c>
       <c r="AE30" s="0">
-        <v>1.02</v>
+        <v>1.03</v>
       </c>
       <c r="AF30" s="0">
-        <v>-0.11</v>
+        <v>0.01</v>
       </c>
       <c r="AG30" s="0">
         <v>0.02</v>
@@ -4096,67 +4084,67 @@
         <v>97</v>
       </c>
       <c r="N31" s="0">
-        <v>567.801</v>
+        <v>551.625</v>
       </c>
       <c r="O31" s="0">
-        <v>75</v>
+        <v>91.76</v>
       </c>
       <c r="P31" s="0">
         <v>0</v>
       </c>
       <c r="Q31" s="0">
-        <v>1.65619</v>
+        <v>1.89833</v>
       </c>
       <c r="R31" s="0">
-        <v>1.99113</v>
+        <v>1.94113</v>
       </c>
       <c r="S31" s="0">
         <v>0</v>
       </c>
       <c r="T31" s="0">
-        <v>540</v>
+        <v>353</v>
       </c>
       <c r="U31" s="0">
-        <v>392</v>
+        <v>205</v>
       </c>
       <c r="V31" s="0">
-        <v>463</v>
+        <v>390</v>
       </c>
       <c r="W31" s="0">
-        <v>249</v>
+        <v>176</v>
       </c>
       <c r="X31" s="0">
-        <v>10.73</v>
+        <v>8.87</v>
       </c>
       <c r="Y31" s="0">
-        <v>15.45</v>
+        <v>8.94</v>
       </c>
       <c r="Z31" s="0">
-        <v>15.45</v>
+        <v>8.94</v>
       </c>
       <c r="AA31" s="0">
-        <v>-25.299</v>
+        <v>-8.606</v>
       </c>
       <c r="AB31" s="0">
-        <v>-27.337</v>
+        <v>-10.695</v>
       </c>
       <c r="AC31" s="0">
-        <v>0.84</v>
+        <v>2.49</v>
       </c>
       <c r="AD31" s="0">
-        <v>3.03</v>
+        <v>3.17</v>
       </c>
       <c r="AE31" s="0">
-        <v>3.03</v>
+        <v>3.17</v>
       </c>
       <c r="AF31" s="0">
-        <v>-0.49</v>
+        <v>-0.1</v>
       </c>
       <c r="AG31" s="0">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="AH31" s="0">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="AI31" s="0" t="s">
         <v>47</v>
@@ -4203,67 +4191,67 @@
         <v>97</v>
       </c>
       <c r="N32" s="0">
-        <v>681.361</v>
+        <v>661.95</v>
       </c>
       <c r="O32" s="0">
-        <v>70.04</v>
+        <v>88.24</v>
       </c>
       <c r="P32" s="0">
         <v>0</v>
       </c>
       <c r="Q32" s="0">
-        <v>1.85599</v>
+        <v>2.19061</v>
       </c>
       <c r="R32" s="0">
-        <v>2.36555</v>
+        <v>2.30616</v>
       </c>
       <c r="S32" s="0">
         <v>0</v>
       </c>
       <c r="T32" s="0">
-        <v>544</v>
+        <v>344</v>
       </c>
       <c r="U32" s="0">
-        <v>359</v>
+        <v>159</v>
       </c>
       <c r="V32" s="0">
-        <v>425</v>
+        <v>347</v>
       </c>
       <c r="W32" s="0">
-        <v>186</v>
+        <v>108</v>
       </c>
       <c r="X32" s="0">
+        <v>7.43</v>
+      </c>
+      <c r="Y32" s="0">
         <v>9.5</v>
       </c>
-      <c r="Y32" s="0">
-        <v>15.63</v>
-      </c>
       <c r="Z32" s="0">
-        <v>15.63</v>
+        <v>9.5</v>
       </c>
       <c r="AA32" s="0">
-        <v>-29.537</v>
+        <v>-11.227</v>
       </c>
       <c r="AB32" s="0">
-        <v>-31.38</v>
+        <v>-13.14</v>
       </c>
       <c r="AC32" s="0">
-        <v>1.05</v>
+        <v>2.87</v>
       </c>
       <c r="AD32" s="0">
-        <v>3.67</v>
+        <v>3.87</v>
       </c>
       <c r="AE32" s="0">
-        <v>3.67</v>
+        <v>3.87</v>
       </c>
       <c r="AF32" s="0">
-        <v>-0.58</v>
+        <v>-0.14</v>
       </c>
       <c r="AG32" s="0">
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
       <c r="AH32" s="0">
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
       <c r="AI32" s="0" t="s">
         <v>47</v>
@@ -4310,61 +4298,61 @@
         <v>161</v>
       </c>
       <c r="N33" s="0">
-        <v>170.34</v>
+        <v>165.487</v>
       </c>
       <c r="O33" s="0">
-        <v>74.4</v>
+        <v>76</v>
       </c>
       <c r="P33" s="0">
         <v>0</v>
       </c>
       <c r="Q33" s="0">
-        <v>0.49288</v>
+        <v>0.47168</v>
       </c>
       <c r="R33" s="0">
-        <v>0.49358</v>
+        <v>0.48118</v>
       </c>
       <c r="S33" s="0">
         <v>0</v>
       </c>
       <c r="T33" s="0">
-        <v>589</v>
+        <v>567</v>
       </c>
       <c r="U33" s="0">
-        <v>155</v>
+        <v>133</v>
       </c>
       <c r="V33" s="0">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="W33" s="0">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="X33" s="0">
-        <v>9.58</v>
+        <v>9.36</v>
       </c>
       <c r="Y33" s="0">
-        <v>14.86</v>
+        <v>14.2</v>
       </c>
       <c r="Z33" s="0">
-        <v>14.86</v>
+        <v>14.2</v>
       </c>
       <c r="AA33" s="0">
-        <v>-10.318</v>
+        <v>-8.39</v>
       </c>
       <c r="AB33" s="0">
-        <v>-12.25</v>
+        <v>-10.501</v>
       </c>
       <c r="AC33" s="0">
-        <v>1.58</v>
+        <v>1.7</v>
       </c>
       <c r="AD33" s="0">
-        <v>3.23</v>
+        <v>3.24</v>
       </c>
       <c r="AE33" s="0">
-        <v>3.23</v>
+        <v>3.24</v>
       </c>
       <c r="AF33" s="0">
-        <v>-0.26</v>
+        <v>-0.24</v>
       </c>
       <c r="AG33" s="0">
         <v>0.14</v>
@@ -4417,61 +4405,61 @@
         <v>97</v>
       </c>
       <c r="N34" s="0">
-        <v>161.823</v>
+        <v>157.213</v>
       </c>
       <c r="O34" s="0">
-        <v>93.64</v>
+        <v>99.76</v>
       </c>
       <c r="P34" s="0">
         <v>0</v>
       </c>
       <c r="Q34" s="0">
-        <v>0.58933</v>
+        <v>0.58819</v>
       </c>
       <c r="R34" s="0">
-        <v>0.61382</v>
+        <v>0.59841</v>
       </c>
       <c r="S34" s="0">
         <v>0</v>
       </c>
       <c r="T34" s="0">
-        <v>479</v>
+        <v>383</v>
       </c>
       <c r="U34" s="0">
-        <v>271</v>
+        <v>175</v>
       </c>
       <c r="V34" s="0">
-        <v>473</v>
+        <v>424</v>
       </c>
       <c r="W34" s="0">
-        <v>179</v>
+        <v>130</v>
       </c>
       <c r="X34" s="0">
-        <v>8.6</v>
+        <v>7.83</v>
       </c>
       <c r="Y34" s="0">
-        <v>10.15</v>
+        <v>8.4</v>
       </c>
       <c r="Z34" s="0">
-        <v>10.15</v>
+        <v>8.4</v>
       </c>
       <c r="AA34" s="0">
-        <v>-13.775</v>
+        <v>-6.241</v>
       </c>
       <c r="AB34" s="0">
-        <v>-15.809</v>
+        <v>-8.38</v>
       </c>
       <c r="AC34" s="0">
-        <v>2.74</v>
+        <v>3.35</v>
       </c>
       <c r="AD34" s="0">
-        <v>3.6</v>
+        <v>3.65</v>
       </c>
       <c r="AE34" s="0">
-        <v>3.6</v>
+        <v>3.65</v>
       </c>
       <c r="AF34" s="0">
-        <v>-0.07</v>
+        <v>0.07</v>
       </c>
       <c r="AG34" s="0">
         <v>0.17</v>
@@ -4524,61 +4512,61 @@
         <v>46</v>
       </c>
       <c r="N35" s="0">
-        <v>681.361</v>
+        <v>661.95</v>
       </c>
       <c r="O35" s="0">
-        <v>92.4</v>
+        <v>91.96</v>
       </c>
       <c r="P35" s="0">
         <v>0</v>
       </c>
       <c r="Q35" s="0">
-        <v>2.44851</v>
+        <v>2.28296</v>
       </c>
       <c r="R35" s="0">
-        <v>2.25608</v>
+        <v>2.19943</v>
       </c>
       <c r="S35" s="0">
         <v>0</v>
       </c>
       <c r="T35" s="0">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="U35" s="0">
-        <v>-15</v>
+        <v>13</v>
       </c>
       <c r="V35" s="0">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="W35" s="0">
-        <v>-16</v>
+        <v>17</v>
       </c>
       <c r="X35" s="0">
-        <v>5.33</v>
+        <v>5.93</v>
       </c>
       <c r="Y35" s="0">
-        <v>6.3</v>
+        <v>6.78</v>
       </c>
       <c r="Z35" s="0">
-        <v>6.3</v>
+        <v>6.78</v>
       </c>
       <c r="AA35" s="0">
-        <v>-1.01</v>
+        <v>-1.474</v>
       </c>
       <c r="AB35" s="0">
-        <v>-1.746</v>
+        <v>-2.317</v>
       </c>
       <c r="AC35" s="0">
-        <v>0.99</v>
+        <v>3.02</v>
       </c>
       <c r="AD35" s="0">
-        <v>0.02</v>
+        <v>0.18</v>
       </c>
       <c r="AE35" s="0">
-        <v>0.02</v>
+        <v>0.18</v>
       </c>
       <c r="AF35" s="0">
-        <v>8.98</v>
+        <v>18.72</v>
       </c>
       <c r="AG35" s="0">
         <v>0</v>
@@ -4631,37 +4619,37 @@
         <v>146</v>
       </c>
       <c r="N36" s="0">
-        <v>888.447</v>
+        <v>915.803</v>
       </c>
       <c r="O36" s="0">
-        <v>77.16</v>
+        <v>80.6</v>
       </c>
       <c r="P36" s="0">
         <v>0</v>
       </c>
       <c r="Q36" s="0">
-        <v>2.6661</v>
+        <v>2.76829</v>
       </c>
       <c r="R36" s="0">
-        <v>2.6116</v>
+        <v>2.70138</v>
       </c>
       <c r="S36" s="0">
         <v>0</v>
       </c>
       <c r="T36" s="0">
-        <v>178</v>
+        <v>138</v>
       </c>
       <c r="U36" s="0">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="V36" s="0">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="W36" s="0">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="X36" s="0">
-        <v>7</v>
+        <v>6.9</v>
       </c>
       <c r="Y36" s="0">
         <v>7.31</v>
@@ -4670,22 +4658,22 @@
         <v>7.31</v>
       </c>
       <c r="AA36" s="0">
-        <v>-8.317</v>
+        <v>-2.599</v>
       </c>
       <c r="AB36" s="0">
-        <v>-9.102</v>
+        <v>-3.356</v>
       </c>
       <c r="AC36" s="0">
-        <v>4.4</v>
+        <v>4.59</v>
       </c>
       <c r="AD36" s="0">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="AE36" s="0">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="AF36" s="0">
-        <v>35.14</v>
+        <v>32.98</v>
       </c>
       <c r="AG36" s="0">
         <v>0</v>
@@ -4738,61 +4726,61 @@
         <v>146</v>
       </c>
       <c r="N37" s="0">
-        <v>807.679</v>
+        <v>832.548</v>
       </c>
       <c r="O37" s="0">
-        <v>95.2</v>
+        <v>98</v>
       </c>
       <c r="P37" s="0">
         <v>0</v>
       </c>
       <c r="Q37" s="0">
-        <v>2.9904</v>
+        <v>3.05992</v>
       </c>
       <c r="R37" s="0">
-        <v>2.82667</v>
+        <v>2.92384</v>
       </c>
       <c r="S37" s="0">
         <v>0</v>
       </c>
       <c r="T37" s="0">
-        <v>300</v>
+        <v>240</v>
       </c>
       <c r="U37" s="0">
-        <v>135</v>
+        <v>75</v>
       </c>
       <c r="V37" s="0">
-        <v>345</v>
+        <v>299</v>
       </c>
       <c r="W37" s="0">
-        <v>119</v>
+        <v>73</v>
       </c>
       <c r="X37" s="0">
-        <v>7.99</v>
+        <v>7.66</v>
       </c>
       <c r="Y37" s="0">
-        <v>7.23</v>
+        <v>6.4</v>
       </c>
       <c r="Z37" s="0">
-        <v>7.23</v>
+        <v>6.4</v>
       </c>
       <c r="AA37" s="0">
-        <v>-4.99</v>
+        <v>-0.736</v>
       </c>
       <c r="AB37" s="0">
-        <v>-7.095</v>
+        <v>-2.91</v>
       </c>
       <c r="AC37" s="0">
-        <v>3.01</v>
+        <v>3.41</v>
       </c>
       <c r="AD37" s="0">
-        <v>3.5</v>
+        <v>3.52</v>
       </c>
       <c r="AE37" s="0">
-        <v>3.5</v>
+        <v>3.52</v>
       </c>
       <c r="AF37" s="0">
-        <v>-0</v>
+        <v>0.12</v>
       </c>
       <c r="AG37" s="0">
         <v>0.16</v>
@@ -4845,52 +4833,52 @@
         <v>146</v>
       </c>
       <c r="N38" s="0">
-        <v>807.679</v>
+        <v>832.548</v>
       </c>
       <c r="O38" s="0">
-        <v>99.68</v>
+        <v>98.8</v>
       </c>
       <c r="P38" s="0">
         <v>0</v>
       </c>
       <c r="Q38" s="0">
-        <v>3.13112</v>
+        <v>3.0849</v>
       </c>
       <c r="R38" s="0">
-        <v>2.86278</v>
+        <v>2.96119</v>
       </c>
       <c r="S38" s="0">
         <v>0</v>
       </c>
       <c r="T38" s="0">
-        <v>292</v>
+        <v>263</v>
       </c>
       <c r="U38" s="0">
-        <v>189</v>
+        <v>160</v>
       </c>
       <c r="V38" s="0">
-        <v>346</v>
+        <v>301</v>
       </c>
       <c r="W38" s="0">
-        <v>227</v>
+        <v>182</v>
       </c>
       <c r="X38" s="0">
-        <v>8.1</v>
+        <v>8.19</v>
       </c>
       <c r="Y38" s="0">
-        <v>6.48</v>
+        <v>7.1</v>
       </c>
       <c r="Z38" s="0">
-        <v>6.48</v>
+        <v>7.1</v>
       </c>
       <c r="AA38" s="0">
-        <v>-1.774</v>
+        <v>-1.07</v>
       </c>
       <c r="AB38" s="0">
-        <v>-2.895</v>
+        <v>-2.234</v>
       </c>
       <c r="AC38" s="0">
-        <v>1.25</v>
+        <v>1.39</v>
       </c>
       <c r="AD38" s="0">
         <v>1.44</v>
@@ -4899,7 +4887,7 @@
         <v>1.44</v>
       </c>
       <c r="AF38" s="0">
-        <v>-0.04</v>
+        <v>0.01</v>
       </c>
       <c r="AG38" s="0">
         <v>0.03</v>
@@ -4952,67 +4940,67 @@
         <v>97</v>
       </c>
       <c r="N39" s="0">
-        <v>283.9</v>
+        <v>275.812</v>
       </c>
       <c r="O39" s="0">
-        <v>93.96</v>
+        <v>98.36</v>
       </c>
       <c r="P39" s="0">
         <v>0</v>
       </c>
       <c r="Q39" s="0">
-        <v>1.03744</v>
+        <v>1.01743</v>
       </c>
       <c r="R39" s="0">
-        <v>1.00349</v>
+        <v>0.9783</v>
       </c>
       <c r="S39" s="0">
         <v>0</v>
       </c>
       <c r="T39" s="0">
-        <v>321</v>
+        <v>232</v>
       </c>
       <c r="U39" s="0">
-        <v>238</v>
+        <v>149</v>
       </c>
       <c r="V39" s="0">
-        <v>374</v>
+        <v>306</v>
       </c>
       <c r="W39" s="0">
-        <v>234</v>
+        <v>166</v>
       </c>
       <c r="X39" s="0">
-        <v>8.13</v>
+        <v>7.37</v>
       </c>
       <c r="Y39" s="0">
-        <v>7.66</v>
+        <v>6.25</v>
       </c>
       <c r="Z39" s="0">
-        <v>7.66</v>
+        <v>6.25</v>
       </c>
       <c r="AA39" s="0">
-        <v>-7.154</v>
+        <v>-2.806</v>
       </c>
       <c r="AB39" s="0">
-        <v>-9.211</v>
+        <v>-4.913</v>
       </c>
       <c r="AC39" s="0">
-        <v>2.85</v>
+        <v>3.17</v>
       </c>
       <c r="AD39" s="0">
-        <v>3.22</v>
+        <v>3.26</v>
       </c>
       <c r="AE39" s="0">
-        <v>3.22</v>
+        <v>3.26</v>
       </c>
       <c r="AF39" s="0">
-        <v>0.01</v>
+        <v>0.11</v>
       </c>
       <c r="AG39" s="0">
-        <v>0.13</v>
+        <v>0.14</v>
       </c>
       <c r="AH39" s="0">
-        <v>0.13</v>
+        <v>0.14</v>
       </c>
       <c r="AI39" s="0" t="s">
         <v>47</v>
@@ -5059,19 +5047,19 @@
         <v>57</v>
       </c>
       <c r="N40" s="0">
-        <v>377.162</v>
+        <v>381.942</v>
       </c>
       <c r="O40" s="0">
-        <v>90.44</v>
+        <v>91.8</v>
       </c>
       <c r="P40" s="0">
         <v>0</v>
       </c>
       <c r="Q40" s="0">
-        <v>1.32661</v>
+        <v>1.31497</v>
       </c>
       <c r="R40" s="0">
-        <v>1.29837</v>
+        <v>1.3194</v>
       </c>
       <c r="S40" s="0">
         <v>0</v>
@@ -5098,10 +5086,10 @@
         <v>24.48</v>
       </c>
       <c r="AA40" s="0">
-        <v>-8.239</v>
+        <v>-6.859</v>
       </c>
       <c r="AB40" s="0">
-        <v>-8.3</v>
+        <v>-7.179</v>
       </c>
       <c r="AC40" s="0">
         <v>-0.5</v>
@@ -5116,9 +5104,6 @@
         <v>-0.2</v>
       </c>
       <c r="AG40" s="0">
-        <v>0</v>
-      </c>
-      <c r="AH40" s="0">
         <v>0</v>
       </c>
       <c r="AI40" s="0" t="s">
@@ -5166,61 +5151,61 @@
         <v>57</v>
       </c>
       <c r="N41" s="0">
-        <v>392.692</v>
+        <v>397.669</v>
       </c>
       <c r="O41" s="0">
-        <v>90.4</v>
+        <v>89.96</v>
       </c>
       <c r="P41" s="0">
         <v>0</v>
       </c>
       <c r="Q41" s="0">
-        <v>1.38062</v>
+        <v>1.34167</v>
       </c>
       <c r="R41" s="0">
-        <v>1.33866</v>
+        <v>1.36034</v>
       </c>
       <c r="S41" s="0">
         <v>0</v>
       </c>
       <c r="T41" s="0">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="U41" s="0">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="V41" s="0">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="W41" s="0">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="X41" s="0">
-        <v>9.59</v>
+        <v>9.93</v>
       </c>
       <c r="Y41" s="0">
-        <v>15.67</v>
+        <v>16.1</v>
       </c>
       <c r="Z41" s="0">
-        <v>15.67</v>
+        <v>16.1</v>
       </c>
       <c r="AA41" s="0">
-        <v>-7.377</v>
+        <v>-7.828</v>
       </c>
       <c r="AB41" s="0">
-        <v>-8.246</v>
+        <v>-8.765</v>
       </c>
       <c r="AC41" s="0">
-        <v>-0.07</v>
+        <v>-0.09</v>
       </c>
       <c r="AD41" s="0">
-        <v>1.12</v>
+        <v>1.11</v>
       </c>
       <c r="AE41" s="0">
-        <v>1.12</v>
+        <v>1.11</v>
       </c>
       <c r="AF41" s="0">
-        <v>-0.26</v>
+        <v>-0.27</v>
       </c>
       <c r="AG41" s="0">
         <v>0.02</v>
@@ -5273,19 +5258,19 @@
         <v>57</v>
       </c>
       <c r="N42" s="0">
-        <v>638.957</v>
+        <v>647.055</v>
       </c>
       <c r="O42" s="0">
-        <v>94.4</v>
+        <v>96.57</v>
       </c>
       <c r="P42" s="0">
         <v>0</v>
       </c>
       <c r="Q42" s="0">
-        <v>2.34583</v>
+        <v>2.34336</v>
       </c>
       <c r="R42" s="0">
-        <v>2.2353</v>
+        <v>2.2715</v>
       </c>
       <c r="S42" s="0">
         <v>0</v>
@@ -5312,10 +5297,10 @@
         <v>41.35</v>
       </c>
       <c r="AA42" s="0">
-        <v>-5.751</v>
+        <v>-3.588</v>
       </c>
       <c r="AB42" s="0">
-        <v>-5.746</v>
+        <v>-3.855</v>
       </c>
       <c r="AC42" s="0">
         <v>-0.7</v>
@@ -5377,67 +5362,67 @@
         <v>134</v>
       </c>
       <c r="N43" s="0">
-        <v>457.08</v>
+        <v>444.058</v>
       </c>
       <c r="O43" s="0">
-        <v>101.44</v>
+        <v>100.48</v>
       </c>
       <c r="P43" s="0">
         <v>0</v>
       </c>
       <c r="Q43" s="0">
-        <v>1.80324</v>
+        <v>1.67338</v>
       </c>
       <c r="R43" s="0">
-        <v>1.65394</v>
+        <v>1.61241</v>
       </c>
       <c r="S43" s="0">
         <v>0</v>
       </c>
       <c r="T43" s="0">
-        <v>-346</v>
+        <v>-176</v>
       </c>
       <c r="U43" s="0">
-        <v>0</v>
+        <v>170</v>
       </c>
       <c r="V43" s="0">
-        <v>-501</v>
+        <v>-156</v>
       </c>
       <c r="W43" s="0">
-        <v>0</v>
+        <v>345</v>
       </c>
       <c r="X43" s="0">
-        <v>1.66</v>
+        <v>3.63</v>
       </c>
       <c r="Y43" s="0">
-        <v>-0.6</v>
+        <v>0.01</v>
       </c>
       <c r="Z43" s="0">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="AA43" s="0">
-        <v>-2.085</v>
+        <v>-0.221</v>
       </c>
       <c r="AB43" s="0">
-        <v>-2.438</v>
+        <v>-0.739</v>
       </c>
       <c r="AC43" s="0">
-        <v>0.35</v>
+        <v>0.01</v>
       </c>
       <c r="AD43" s="0">
-        <v>0.09</v>
+        <v>19.22</v>
       </c>
       <c r="AE43" s="0">
-        <v>0.09</v>
+        <v>19.22</v>
       </c>
       <c r="AF43" s="0">
-        <v>-0.22</v>
+        <v>-0.06</v>
       </c>
       <c r="AG43" s="0">
-        <v>0</v>
+        <v>3.81</v>
       </c>
       <c r="AH43" s="0">
-        <v>0</v>
+        <v>3.81</v>
       </c>
       <c r="AI43" s="0" t="s">
         <v>72</v>
@@ -5484,61 +5469,61 @@
         <v>134</v>
       </c>
       <c r="N44" s="0">
-        <v>437.207</v>
+        <v>424.751</v>
       </c>
       <c r="O44" s="0">
-        <v>89.6</v>
+        <v>91.08</v>
       </c>
       <c r="P44" s="0">
         <v>0</v>
       </c>
       <c r="Q44" s="0">
-        <v>1.52352</v>
+        <v>1.45088</v>
       </c>
       <c r="R44" s="0">
-        <v>1.48491</v>
+        <v>1.44763</v>
       </c>
       <c r="S44" s="0">
         <v>0</v>
       </c>
       <c r="T44" s="0">
-        <v>526</v>
+        <v>599</v>
       </c>
       <c r="U44" s="0">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="V44" s="0">
-        <v>551</v>
+        <v>583</v>
       </c>
       <c r="W44" s="0">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="X44" s="0">
-        <v>10.47</v>
+        <v>11.8</v>
       </c>
       <c r="Y44" s="0">
-        <v>10.93</v>
+        <v>12.05</v>
       </c>
       <c r="Z44" s="0">
-        <v>10.93</v>
+        <v>12.05</v>
       </c>
       <c r="AA44" s="0">
-        <v>-7.857</v>
+        <v>-6.335</v>
       </c>
       <c r="AB44" s="0">
-        <v>-7.821</v>
+        <v>-6.571</v>
       </c>
       <c r="AC44" s="0">
-        <v>-0.69</v>
+        <v>-1.1</v>
       </c>
       <c r="AD44" s="0">
-        <v>0.04</v>
+        <v>0.17</v>
       </c>
       <c r="AE44" s="0">
-        <v>0.04</v>
+        <v>0.17</v>
       </c>
       <c r="AF44" s="0">
-        <v>-0.17</v>
+        <v>-0.25</v>
       </c>
       <c r="AG44" s="0">
         <v>0</v>
@@ -5591,19 +5576,19 @@
         <v>134</v>
       </c>
       <c r="N45" s="0">
-        <v>195.891</v>
+        <v>190.311</v>
       </c>
       <c r="O45" s="0">
-        <v>97.72</v>
+        <v>101</v>
       </c>
       <c r="P45" s="0">
         <v>0</v>
       </c>
       <c r="Q45" s="0">
-        <v>0.74448</v>
+        <v>0.72087</v>
       </c>
       <c r="R45" s="0">
-        <v>0.69433</v>
+        <v>0.6769</v>
       </c>
       <c r="S45" s="0">
         <v>0</v>
@@ -5630,10 +5615,10 @@
         <v>99.99</v>
       </c>
       <c r="AA45" s="0">
-        <v>-3.705</v>
+        <v>-0.473</v>
       </c>
       <c r="AB45" s="0">
-        <v>-3.665</v>
+        <v>-0.7</v>
       </c>
       <c r="AC45" s="0">
         <v>-0.66</v>
@@ -5698,67 +5683,67 @@
         <v>97</v>
       </c>
       <c r="N46" s="0">
-        <v>584.835</v>
+        <v>568.174</v>
       </c>
       <c r="O46" s="0">
-        <v>70.4</v>
+        <v>91.04</v>
       </c>
       <c r="P46" s="0">
         <v>0</v>
       </c>
       <c r="Q46" s="0">
-        <v>1.60125</v>
+        <v>1.93994</v>
       </c>
       <c r="R46" s="0">
-        <v>2.02145</v>
+        <v>1.97069</v>
       </c>
       <c r="S46" s="0">
         <v>0</v>
       </c>
       <c r="T46" s="0">
-        <v>601</v>
+        <v>363</v>
       </c>
       <c r="U46" s="0">
-        <v>354</v>
+        <v>116</v>
       </c>
       <c r="V46" s="0">
-        <v>476</v>
+        <v>392</v>
       </c>
       <c r="W46" s="0">
-        <v>167</v>
+        <v>83</v>
       </c>
       <c r="X46" s="0">
-        <v>11.39</v>
+        <v>8.97</v>
       </c>
       <c r="Y46" s="0">
-        <v>17.21</v>
+        <v>9.28</v>
       </c>
       <c r="Z46" s="0">
-        <v>17.21</v>
+        <v>9.28</v>
       </c>
       <c r="AA46" s="0">
-        <v>-27.25</v>
+        <v>-6.393</v>
       </c>
       <c r="AB46" s="0">
-        <v>-29.264</v>
+        <v>-8.482</v>
       </c>
       <c r="AC46" s="0">
-        <v>0.51</v>
+        <v>2.54</v>
       </c>
       <c r="AD46" s="0">
-        <v>3.15</v>
+        <v>3.35</v>
       </c>
       <c r="AE46" s="0">
-        <v>3.15</v>
+        <v>3.35</v>
       </c>
       <c r="AF46" s="0">
-        <v>-0.58</v>
+        <v>-0.12</v>
       </c>
       <c r="AG46" s="0">
-        <v>0.13</v>
+        <v>0.15</v>
       </c>
       <c r="AH46" s="0">
-        <v>0.13</v>
+        <v>0.15</v>
       </c>
       <c r="AI46" s="0" t="s">
         <v>47</v>
@@ -5805,67 +5790,67 @@
         <v>97</v>
       </c>
       <c r="N47" s="0">
-        <v>582.847</v>
+        <v>566.243</v>
       </c>
       <c r="O47" s="0">
-        <v>34.8</v>
+        <v>60</v>
       </c>
       <c r="P47" s="0">
         <v>0</v>
       </c>
       <c r="Q47" s="0">
-        <v>0.78884</v>
+        <v>1.27417</v>
       </c>
       <c r="R47" s="0">
-        <v>2.06995</v>
+        <v>2.01797</v>
       </c>
       <c r="S47" s="0">
         <v>0</v>
       </c>
       <c r="T47" s="0">
-        <v>1968</v>
+        <v>974</v>
       </c>
       <c r="U47" s="0">
-        <v>1696</v>
+        <v>702</v>
       </c>
       <c r="V47" s="0">
-        <v>716</v>
+        <v>621</v>
       </c>
       <c r="W47" s="0">
-        <v>358</v>
+        <v>263</v>
       </c>
       <c r="X47" s="0">
-        <v>23.5</v>
+        <v>13.75</v>
       </c>
       <c r="Y47" s="0">
-        <v>42.19</v>
+        <v>23.14</v>
       </c>
       <c r="Z47" s="0">
-        <v>42.19</v>
+        <v>23.14</v>
       </c>
       <c r="AA47" s="0">
-        <v>-65.775</v>
+        <v>-40.991</v>
       </c>
       <c r="AB47" s="0">
-        <v>-67.776</v>
+        <v>-43.071</v>
       </c>
       <c r="AC47" s="0">
-        <v>-0.41</v>
+        <v>0.57</v>
       </c>
       <c r="AD47" s="0">
-        <v>2.58</v>
+        <v>3.14</v>
       </c>
       <c r="AE47" s="0">
-        <v>2.58</v>
+        <v>3.14</v>
       </c>
       <c r="AF47" s="0">
-        <v>-0.4</v>
+        <v>-0.46</v>
       </c>
       <c r="AG47" s="0">
-        <v>0.1</v>
+        <v>0.14</v>
       </c>
       <c r="AH47" s="0">
-        <v>0.1</v>
+        <v>0.14</v>
       </c>
       <c r="AI47" s="0" t="s">
         <v>47</v>
@@ -5912,67 +5897,67 @@
         <v>97</v>
       </c>
       <c r="N48" s="0">
-        <v>567.801</v>
+        <v>551.625</v>
       </c>
       <c r="O48" s="0">
-        <v>77.28</v>
+        <v>84.4</v>
       </c>
       <c r="P48" s="0">
         <v>0</v>
       </c>
       <c r="Q48" s="0">
-        <v>1.70654</v>
+        <v>1.74607</v>
       </c>
       <c r="R48" s="0">
-        <v>1.95146</v>
+        <v>1.90246</v>
       </c>
       <c r="S48" s="0">
         <v>0</v>
       </c>
       <c r="T48" s="0">
-        <v>421</v>
+        <v>347</v>
       </c>
       <c r="U48" s="0">
-        <v>246</v>
+        <v>172</v>
       </c>
       <c r="V48" s="0">
-        <v>381</v>
+        <v>353</v>
       </c>
       <c r="W48" s="0">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="X48" s="0">
-        <v>9.17</v>
+        <v>8.59</v>
       </c>
       <c r="Y48" s="0">
-        <v>10.99</v>
+        <v>9.21</v>
       </c>
       <c r="Z48" s="0">
-        <v>10.99</v>
+        <v>9.21</v>
       </c>
       <c r="AA48" s="0">
-        <v>-21.463</v>
+        <v>-14.228</v>
       </c>
       <c r="AB48" s="0">
-        <v>-24.003</v>
+        <v>-16.88</v>
       </c>
       <c r="AC48" s="0">
-        <v>3.07</v>
+        <v>3.76</v>
       </c>
       <c r="AD48" s="0">
-        <v>4.89</v>
+        <v>5</v>
       </c>
       <c r="AE48" s="0">
-        <v>4.89</v>
+        <v>5</v>
       </c>
       <c r="AF48" s="0">
-        <v>-0.31</v>
+        <v>-0.14</v>
       </c>
       <c r="AG48" s="0">
-        <v>0.31</v>
+        <v>0.32</v>
       </c>
       <c r="AH48" s="0">
-        <v>0.31</v>
+        <v>0.32</v>
       </c>
       <c r="AI48" s="0" t="s">
         <v>47</v>
@@ -6019,67 +6004,67 @@
         <v>97</v>
       </c>
       <c r="N49" s="0">
-        <v>567.801</v>
+        <v>551.625</v>
       </c>
       <c r="O49" s="0">
-        <v>78.4</v>
+        <v>93.92</v>
       </c>
       <c r="P49" s="0">
         <v>0</v>
       </c>
       <c r="Q49" s="0">
-        <v>1.73127</v>
+        <v>1.94302</v>
       </c>
       <c r="R49" s="0">
-        <v>2.03079</v>
+        <v>1.9798</v>
       </c>
       <c r="S49" s="0">
         <v>0</v>
       </c>
       <c r="T49" s="0">
-        <v>485</v>
+        <v>316</v>
       </c>
       <c r="U49" s="0">
-        <v>527</v>
+        <v>358</v>
       </c>
       <c r="V49" s="0">
-        <v>426</v>
+        <v>355</v>
       </c>
       <c r="W49" s="0">
-        <v>583</v>
+        <v>512</v>
       </c>
       <c r="X49" s="0">
-        <v>10.53</v>
+        <v>8.83</v>
       </c>
       <c r="Y49" s="0">
-        <v>25.49</v>
+        <v>11.33</v>
       </c>
       <c r="Z49" s="0">
-        <v>25.49</v>
+        <v>11.33</v>
       </c>
       <c r="AA49" s="0">
-        <v>-23.438</v>
+        <v>-8.281</v>
       </c>
       <c r="AB49" s="0">
-        <v>-24.512</v>
+        <v>-9.397</v>
       </c>
       <c r="AC49" s="0">
-        <v>-1.37</v>
+        <v>0.5</v>
       </c>
       <c r="AD49" s="0">
-        <v>1.23</v>
+        <v>1.32</v>
       </c>
       <c r="AE49" s="0">
-        <v>1.23</v>
+        <v>1.32</v>
       </c>
       <c r="AF49" s="0">
-        <v>-0.61</v>
+        <v>-0.22</v>
       </c>
       <c r="AG49" s="0">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="AH49" s="0">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="AI49" s="0" t="s">
         <v>47</v>
@@ -6126,61 +6111,61 @@
         <v>128</v>
       </c>
       <c r="N50" s="0">
-        <v>414.082</v>
+        <v>423.074</v>
       </c>
       <c r="O50" s="0">
-        <v>98.76</v>
+        <v>101.4</v>
       </c>
       <c r="P50" s="0">
         <v>0</v>
       </c>
       <c r="Q50" s="0">
-        <v>1.59045</v>
+        <v>1.6089</v>
       </c>
       <c r="R50" s="0">
-        <v>1.49084</v>
+        <v>1.52851</v>
       </c>
       <c r="S50" s="0">
         <v>0</v>
       </c>
       <c r="T50" s="0">
-        <v>214</v>
+        <v>130</v>
       </c>
       <c r="U50" s="0">
-        <v>211</v>
+        <v>127</v>
       </c>
       <c r="V50" s="0">
-        <v>282</v>
+        <v>192</v>
       </c>
       <c r="W50" s="0">
-        <v>263</v>
+        <v>173</v>
       </c>
       <c r="X50" s="0">
-        <v>7.1</v>
+        <v>6.41</v>
       </c>
       <c r="Y50" s="0">
-        <v>6.32</v>
+        <v>5.39</v>
       </c>
       <c r="Z50" s="0">
-        <v>6.32</v>
+        <v>5.39</v>
       </c>
       <c r="AA50" s="0">
-        <v>-4.191</v>
+        <v>-1.63</v>
       </c>
       <c r="AB50" s="0">
-        <v>-6.113</v>
+        <v>-3.583</v>
       </c>
       <c r="AC50" s="0">
-        <v>2.74</v>
+        <v>2.82</v>
       </c>
       <c r="AD50" s="0">
-        <v>2.85</v>
+        <v>2.87</v>
       </c>
       <c r="AE50" s="0">
-        <v>2.85</v>
+        <v>2.87</v>
       </c>
       <c r="AF50" s="0">
-        <v>0.08</v>
+        <v>0.07</v>
       </c>
       <c r="AG50" s="0">
         <v>0.11</v>
@@ -6233,61 +6218,61 @@
         <v>128</v>
       </c>
       <c r="N51" s="0">
-        <v>724.643</v>
+        <v>740.38</v>
       </c>
       <c r="O51" s="0">
-        <v>103.24</v>
+        <v>104.12</v>
       </c>
       <c r="P51" s="0">
         <v>0</v>
       </c>
       <c r="Q51" s="0">
-        <v>2.90955</v>
+        <v>2.8911</v>
       </c>
       <c r="R51" s="0">
-        <v>2.66565</v>
+        <v>2.73302</v>
       </c>
       <c r="S51" s="0">
         <v>0</v>
       </c>
       <c r="T51" s="0">
-        <v>251</v>
+        <v>201</v>
       </c>
       <c r="U51" s="0">
-        <v>92</v>
+        <v>42</v>
       </c>
       <c r="V51" s="0">
-        <v>285</v>
+        <v>247</v>
       </c>
       <c r="W51" s="0">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="X51" s="0">
-        <v>6.16</v>
+        <v>5.79</v>
       </c>
       <c r="Y51" s="0">
-        <v>6.28</v>
+        <v>6.06</v>
       </c>
       <c r="Z51" s="0">
-        <v>6.28</v>
+        <v>6.06</v>
       </c>
       <c r="AA51" s="0">
-        <v>-1.975</v>
+        <v>0.552</v>
       </c>
       <c r="AB51" s="0">
-        <v>-4.138</v>
+        <v>-1.724</v>
       </c>
       <c r="AC51" s="0">
-        <v>3.55</v>
+        <v>3.71</v>
       </c>
       <c r="AD51" s="0">
-        <v>3.82</v>
+        <v>3.83</v>
       </c>
       <c r="AE51" s="0">
-        <v>3.82</v>
+        <v>3.83</v>
       </c>
       <c r="AF51" s="0">
-        <v>0.12</v>
+        <v>0.15</v>
       </c>
       <c r="AG51" s="0">
         <v>0.19</v>
@@ -6340,61 +6325,61 @@
         <v>57</v>
       </c>
       <c r="N52" s="0">
-        <v>452.196</v>
+        <v>439.314</v>
       </c>
       <c r="O52" s="0">
-        <v>71.6</v>
+        <v>73.44</v>
       </c>
       <c r="P52" s="0">
         <v>0</v>
       </c>
       <c r="Q52" s="0">
-        <v>1.2592</v>
+        <v>1.20999</v>
       </c>
       <c r="R52" s="0">
-        <v>1.29449</v>
+        <v>1.26198</v>
       </c>
       <c r="S52" s="0">
         <v>0</v>
       </c>
       <c r="T52" s="0">
-        <v>738</v>
+        <v>698</v>
       </c>
       <c r="U52" s="0">
-        <v>188</v>
+        <v>148</v>
       </c>
       <c r="V52" s="0">
-        <v>582</v>
+        <v>572</v>
       </c>
       <c r="W52" s="0">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="X52" s="0">
-        <v>12.82</v>
+        <v>12.77</v>
       </c>
       <c r="Y52" s="0">
-        <v>27.59</v>
+        <v>25.94</v>
       </c>
       <c r="Z52" s="0">
-        <v>27.59</v>
+        <v>25.94</v>
       </c>
       <c r="AA52" s="0">
-        <v>-12.64</v>
+        <v>-10.395</v>
       </c>
       <c r="AB52" s="0">
-        <v>-13.565</v>
+        <v>-11.447</v>
       </c>
       <c r="AC52" s="0">
-        <v>-1.04</v>
+        <v>-0.86</v>
       </c>
       <c r="AD52" s="0">
-        <v>1.53</v>
+        <v>1.54</v>
       </c>
       <c r="AE52" s="0">
-        <v>1.53</v>
+        <v>1.54</v>
       </c>
       <c r="AF52" s="0">
-        <v>-0.49</v>
+        <v>-0.47</v>
       </c>
       <c r="AG52" s="0">
         <v>0.04</v>
@@ -6447,61 +6432,61 @@
         <v>57</v>
       </c>
       <c r="N53" s="0">
-        <v>528.055</v>
+        <v>513.011</v>
       </c>
       <c r="O53" s="0">
-        <v>75</v>
+        <v>77.8</v>
       </c>
       <c r="P53" s="0">
         <v>0</v>
       </c>
       <c r="Q53" s="0">
-        <v>1.54026</v>
+        <v>1.49686</v>
       </c>
       <c r="R53" s="0">
-        <v>1.59501</v>
+        <v>1.55496</v>
       </c>
       <c r="S53" s="0">
         <v>0</v>
       </c>
       <c r="T53" s="0">
-        <v>783</v>
+        <v>733</v>
       </c>
       <c r="U53" s="0">
-        <v>225</v>
+        <v>175</v>
       </c>
       <c r="V53" s="0">
-        <v>676</v>
+        <v>654</v>
       </c>
       <c r="W53" s="0">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="X53" s="0">
-        <v>11.68</v>
+        <v>11.21</v>
       </c>
       <c r="Y53" s="0">
-        <v>17.01</v>
+        <v>15.74</v>
       </c>
       <c r="Z53" s="0">
-        <v>17.01</v>
+        <v>15.74</v>
       </c>
       <c r="AA53" s="0">
-        <v>-13.275</v>
+        <v>-10.037</v>
       </c>
       <c r="AB53" s="0">
-        <v>-14.949</v>
+        <v>-11.656</v>
       </c>
       <c r="AC53" s="0">
-        <v>1.54</v>
+        <v>1.7</v>
       </c>
       <c r="AD53" s="0">
-        <v>2.87</v>
+        <v>2.9</v>
       </c>
       <c r="AE53" s="0">
-        <v>2.87</v>
+        <v>2.9</v>
       </c>
       <c r="AF53" s="0">
-        <v>-0.21</v>
+        <v>-0.17</v>
       </c>
       <c r="AG53" s="0">
         <v>0.11</v>
@@ -6554,61 +6539,61 @@
         <v>57</v>
       </c>
       <c r="N54" s="0">
-        <v>320.807</v>
+        <v>311.668</v>
       </c>
       <c r="O54" s="0">
-        <v>84.16</v>
+        <v>82.2</v>
       </c>
       <c r="P54" s="0">
         <v>0</v>
       </c>
       <c r="Q54" s="0">
-        <v>1.05003</v>
+        <v>0.96081</v>
       </c>
       <c r="R54" s="0">
-        <v>1.02459</v>
+        <v>0.99886</v>
       </c>
       <c r="S54" s="0">
         <v>0</v>
       </c>
       <c r="T54" s="0">
-        <v>644</v>
+        <v>667</v>
       </c>
       <c r="U54" s="0">
-        <v>145</v>
+        <v>168</v>
       </c>
       <c r="V54" s="0">
-        <v>597</v>
+        <v>606</v>
       </c>
       <c r="W54" s="0">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="X54" s="0">
-        <v>11.66</v>
+        <v>12.32</v>
       </c>
       <c r="Y54" s="0">
-        <v>22.12</v>
+        <v>24.14</v>
       </c>
       <c r="Z54" s="0">
-        <v>22.12</v>
+        <v>24.14</v>
       </c>
       <c r="AA54" s="0">
-        <v>-7.962</v>
+        <v>-10.105</v>
       </c>
       <c r="AB54" s="0">
-        <v>-8.711</v>
+        <v>-10.951</v>
       </c>
       <c r="AC54" s="0">
-        <v>-0.41</v>
+        <v>-0.54</v>
       </c>
       <c r="AD54" s="0">
-        <v>1.17</v>
+        <v>1.16</v>
       </c>
       <c r="AE54" s="0">
-        <v>1.17</v>
+        <v>1.16</v>
       </c>
       <c r="AF54" s="0">
-        <v>-0.31</v>
+        <v>-0.34</v>
       </c>
       <c r="AG54" s="0">
         <v>0.02</v>
@@ -6661,52 +6646,52 @@
         <v>57</v>
       </c>
       <c r="N55" s="0">
-        <v>176.302</v>
+        <v>171.28</v>
       </c>
       <c r="O55" s="0">
-        <v>85.54</v>
+        <v>84.64</v>
       </c>
       <c r="P55" s="0">
         <v>0</v>
       </c>
       <c r="Q55" s="0">
-        <v>0.58652</v>
+        <v>0.5437</v>
       </c>
       <c r="R55" s="0">
-        <v>0.58401</v>
+        <v>0.56934</v>
       </c>
       <c r="S55" s="0">
         <v>0</v>
       </c>
       <c r="T55" s="0">
-        <v>648</v>
+        <v>654</v>
       </c>
       <c r="U55" s="0">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="V55" s="0">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="W55" s="0">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="X55" s="0">
-        <v>11.67</v>
+        <v>12.12</v>
       </c>
       <c r="Y55" s="0">
-        <v>21.22</v>
+        <v>22.12</v>
       </c>
       <c r="Z55" s="0">
-        <v>21.22</v>
+        <v>22.12</v>
       </c>
       <c r="AA55" s="0">
-        <v>-9.806</v>
+        <v>-10.755</v>
       </c>
       <c r="AB55" s="0">
-        <v>-10.645</v>
+        <v>-11.676</v>
       </c>
       <c r="AC55" s="0">
-        <v>-0.29</v>
+        <v>-0.34</v>
       </c>
       <c r="AD55" s="0">
         <v>1.17</v>
@@ -6768,61 +6753,61 @@
         <v>141</v>
       </c>
       <c r="N56" s="0">
-        <v>454.241</v>
+        <v>441.3</v>
       </c>
       <c r="O56" s="0">
-        <v>59.51</v>
+        <v>60</v>
       </c>
       <c r="P56" s="0">
         <v>0</v>
       </c>
       <c r="Q56" s="0">
-        <v>1.05131</v>
+        <v>0.99302</v>
       </c>
       <c r="R56" s="0">
-        <v>1.03015</v>
+        <v>1.00428</v>
       </c>
       <c r="S56" s="0">
         <v>0</v>
       </c>
       <c r="T56" s="0">
-        <v>226</v>
+        <v>255</v>
       </c>
       <c r="U56" s="0">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="V56" s="0">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="W56" s="0">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="X56" s="0">
-        <v>6.41</v>
+        <v>7.21</v>
       </c>
       <c r="Y56" s="0">
-        <v>8.9</v>
+        <v>9.92</v>
       </c>
       <c r="Z56" s="0">
-        <v>8.9</v>
+        <v>9.92</v>
       </c>
       <c r="AA56" s="0">
-        <v>-5.869</v>
+        <v>-5.115</v>
       </c>
       <c r="AB56" s="0">
-        <v>-3.81</v>
+        <v>-3.793</v>
       </c>
       <c r="AC56" s="0">
-        <v>-7.54</v>
+        <v>-8.6</v>
       </c>
       <c r="AD56" s="0">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="AE56" s="0">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="AF56" s="0">
-        <v>-1.56</v>
+        <v>-1.83</v>
       </c>
       <c r="AG56" s="0">
         <v>0</v>
@@ -6875,61 +6860,61 @@
         <v>97</v>
       </c>
       <c r="N57" s="0">
-        <v>397.46</v>
+        <v>386.137</v>
       </c>
       <c r="O57" s="0">
-        <v>65.56</v>
+        <v>83.44</v>
       </c>
       <c r="P57" s="0">
         <v>0</v>
       </c>
       <c r="Q57" s="0">
-        <v>1.01341</v>
+        <v>1.20834</v>
       </c>
       <c r="R57" s="0">
-        <v>1.36602</v>
+        <v>1.33172</v>
       </c>
       <c r="S57" s="0">
         <v>0</v>
       </c>
       <c r="T57" s="0">
-        <v>829</v>
+        <v>553</v>
       </c>
       <c r="U57" s="0">
-        <v>484</v>
+        <v>208</v>
       </c>
       <c r="V57" s="0">
-        <v>529</v>
+        <v>457</v>
       </c>
       <c r="W57" s="0">
-        <v>174</v>
+        <v>102</v>
       </c>
       <c r="X57" s="0">
-        <v>11.84</v>
+        <v>9.28</v>
       </c>
       <c r="Y57" s="0">
-        <v>72.48</v>
+        <v>32.17</v>
       </c>
       <c r="Z57" s="0">
-        <v>72.48</v>
+        <v>32.17</v>
       </c>
       <c r="AA57" s="0">
-        <v>-33.374</v>
+        <v>-13.711</v>
       </c>
       <c r="AB57" s="0">
-        <v>-34.2</v>
+        <v>-14.611</v>
       </c>
       <c r="AC57" s="0">
-        <v>-3.35</v>
+        <v>-1.07</v>
       </c>
       <c r="AD57" s="0">
-        <v>0.62</v>
+        <v>0.79</v>
       </c>
       <c r="AE57" s="0">
-        <v>0.62</v>
+        <v>0.79</v>
       </c>
       <c r="AF57" s="0">
-        <v>-0.71</v>
+        <v>-0.36</v>
       </c>
       <c r="AG57" s="0">
         <v>0.01</v>
@@ -6982,61 +6967,61 @@
         <v>244</v>
       </c>
       <c r="N58" s="0">
-        <v>567.801</v>
+        <v>551.625</v>
       </c>
       <c r="O58" s="0">
-        <v>94.92</v>
+        <v>99.68</v>
       </c>
       <c r="P58" s="0">
         <v>0</v>
       </c>
       <c r="Q58" s="0">
-        <v>2.09608</v>
+        <v>2.06218</v>
       </c>
       <c r="R58" s="0">
-        <v>1.99906</v>
+        <v>1.94886</v>
       </c>
       <c r="S58" s="0">
         <v>0</v>
       </c>
       <c r="T58" s="0">
-        <v>300</v>
+        <v>158</v>
       </c>
       <c r="U58" s="0">
-        <v>256</v>
+        <v>114</v>
       </c>
       <c r="V58" s="0">
-        <v>351</v>
+        <v>227</v>
       </c>
       <c r="W58" s="0">
-        <v>273</v>
+        <v>149</v>
       </c>
       <c r="X58" s="0">
-        <v>8.13</v>
+        <v>6.72</v>
       </c>
       <c r="Y58" s="0">
-        <v>7.44</v>
+        <v>5.59</v>
       </c>
       <c r="Z58" s="0">
-        <v>7.44</v>
+        <v>5.59</v>
       </c>
       <c r="AA58" s="0">
-        <v>-5.833</v>
+        <v>-1.111</v>
       </c>
       <c r="AB58" s="0">
-        <v>-7.683</v>
+        <v>-2.984</v>
       </c>
       <c r="AC58" s="0">
-        <v>2.4</v>
+        <v>2.65</v>
       </c>
       <c r="AD58" s="0">
-        <v>2.64</v>
+        <v>2.67</v>
       </c>
       <c r="AE58" s="0">
-        <v>2.64</v>
+        <v>2.67</v>
       </c>
       <c r="AF58" s="0">
-        <v>0.01</v>
+        <v>0.09</v>
       </c>
       <c r="AG58" s="0">
         <v>0.09</v>
@@ -7089,67 +7074,67 @@
         <v>57</v>
       </c>
       <c r="N59" s="0">
-        <v>335.002</v>
+        <v>325.459</v>
       </c>
       <c r="O59" s="0">
-        <v>81.16</v>
+        <v>79.32</v>
       </c>
       <c r="P59" s="0">
         <v>0</v>
       </c>
       <c r="Q59" s="0">
-        <v>1.05741</v>
+        <v>0.96817</v>
       </c>
       <c r="R59" s="0">
-        <v>1.01563</v>
+        <v>0.99013</v>
       </c>
       <c r="S59" s="0">
         <v>0</v>
       </c>
       <c r="T59" s="0">
-        <v>621</v>
+        <v>641</v>
       </c>
       <c r="U59" s="0">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="V59" s="0">
-        <v>551</v>
+        <v>558</v>
       </c>
       <c r="W59" s="0">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="X59" s="0">
-        <v>11.39</v>
+        <v>12.01</v>
       </c>
       <c r="Y59" s="0">
-        <v>21.34</v>
+        <v>22.85</v>
       </c>
       <c r="Z59" s="0">
-        <v>21.34</v>
+        <v>22.85</v>
       </c>
       <c r="AA59" s="0">
-        <v>-6.498</v>
+        <v>-8.618</v>
       </c>
       <c r="AB59" s="0">
-        <v>-7.444</v>
+        <v>-9.681</v>
       </c>
       <c r="AC59" s="0">
-        <v>-0.41</v>
+        <v>-0.53</v>
       </c>
       <c r="AD59" s="0">
-        <v>1.52</v>
+        <v>1.51</v>
       </c>
       <c r="AE59" s="0">
-        <v>1.52</v>
+        <v>1.51</v>
       </c>
       <c r="AF59" s="0">
         <v>-0.4</v>
       </c>
       <c r="AG59" s="0">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="AH59" s="0">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="AI59" s="0" t="s">
         <v>47</v>
@@ -7196,61 +7181,61 @@
         <v>57</v>
       </c>
       <c r="N60" s="0">
-        <v>326.485</v>
+        <v>317.184</v>
       </c>
       <c r="O60" s="0">
-        <v>77.88</v>
+        <v>77.4</v>
       </c>
       <c r="P60" s="0">
         <v>0</v>
       </c>
       <c r="Q60" s="0">
-        <v>0.98888</v>
+        <v>0.92072</v>
       </c>
       <c r="R60" s="0">
-        <v>0.98114</v>
+        <v>0.95651</v>
       </c>
       <c r="S60" s="0">
         <v>0</v>
       </c>
       <c r="T60" s="0">
-        <v>691</v>
+        <v>695</v>
       </c>
       <c r="U60" s="0">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="V60" s="0">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="W60" s="0">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="X60" s="0">
-        <v>11.75</v>
+        <v>12.06</v>
       </c>
       <c r="Y60" s="0">
-        <v>15.4</v>
+        <v>15.59</v>
       </c>
       <c r="Z60" s="0">
-        <v>15.4</v>
+        <v>15.59</v>
       </c>
       <c r="AA60" s="0">
-        <v>-9.484</v>
+        <v>-10.042</v>
       </c>
       <c r="AB60" s="0">
-        <v>-11.295</v>
+        <v>-12.012</v>
       </c>
       <c r="AC60" s="0">
-        <v>1.72</v>
+        <v>1.69</v>
       </c>
       <c r="AD60" s="0">
-        <v>3.3</v>
+        <v>3.29</v>
       </c>
       <c r="AE60" s="0">
-        <v>3.3</v>
+        <v>3.29</v>
       </c>
       <c r="AF60" s="0">
-        <v>-0.26</v>
+        <v>-0.25</v>
       </c>
       <c r="AG60" s="0">
         <v>0.15</v>
@@ -7303,52 +7288,52 @@
         <v>97</v>
       </c>
       <c r="N61" s="0">
-        <v>959.167</v>
+        <v>1008.554</v>
       </c>
       <c r="O61" s="0">
-        <v>75.48</v>
+        <v>75.44</v>
       </c>
       <c r="P61" s="0">
         <v>0</v>
       </c>
       <c r="Q61" s="0">
-        <v>2.81565</v>
+        <v>2.85348</v>
       </c>
       <c r="R61" s="0">
-        <v>2.79</v>
+        <v>2.94386</v>
       </c>
       <c r="S61" s="0">
         <v>0</v>
       </c>
       <c r="T61" s="0">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="U61" s="0">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="V61" s="0">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="W61" s="0">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="X61" s="0">
-        <v>7.04</v>
+        <v>7.34</v>
       </c>
       <c r="Y61" s="0">
-        <v>7.34</v>
+        <v>7.66</v>
       </c>
       <c r="Z61" s="0">
-        <v>7.34</v>
+        <v>7.66</v>
       </c>
       <c r="AA61" s="0">
-        <v>-9.366</v>
+        <v>-7.784</v>
       </c>
       <c r="AB61" s="0">
-        <v>-10.082</v>
+        <v>-8.566</v>
       </c>
       <c r="AC61" s="0">
-        <v>1.33</v>
+        <v>1.34</v>
       </c>
       <c r="AD61" s="0">
         <v>0</v>
@@ -7357,7 +7342,7 @@
         <v>0</v>
       </c>
       <c r="AF61" s="0">
-        <v>25.31</v>
+        <v>24.66</v>
       </c>
       <c r="AG61" s="0">
         <v>0</v>
@@ -7410,67 +7395,67 @@
         <v>97</v>
       </c>
       <c r="N62" s="0">
-        <v>551.159</v>
+        <v>579.537</v>
       </c>
       <c r="O62" s="0">
-        <v>78.58</v>
+        <v>75.75</v>
       </c>
       <c r="P62" s="0">
         <v>0</v>
       </c>
       <c r="Q62" s="0">
-        <v>1.68435</v>
+        <v>1.64652</v>
       </c>
       <c r="R62" s="0">
-        <v>1.59011</v>
+        <v>1.67779</v>
       </c>
       <c r="S62" s="0">
         <v>0</v>
       </c>
       <c r="T62" s="0">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="U62" s="0">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="V62" s="0">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="W62" s="0">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="X62" s="0">
-        <v>6.22</v>
+        <v>6.77</v>
       </c>
       <c r="Y62" s="0">
-        <v>0.41</v>
+        <v>0.45</v>
       </c>
       <c r="Z62" s="0">
-        <v>0.41</v>
+        <v>0.45</v>
       </c>
       <c r="AA62" s="0">
-        <v>-4.869</v>
+        <v>-6.516</v>
       </c>
       <c r="AB62" s="0">
-        <v>-5.807</v>
+        <v>-7.196</v>
       </c>
       <c r="AC62" s="0">
-        <v>6.81</v>
+        <v>6.45</v>
       </c>
       <c r="AD62" s="0">
-        <v>58.28</v>
+        <v>58.25</v>
       </c>
       <c r="AE62" s="0">
-        <v>58.28</v>
+        <v>58.25</v>
       </c>
       <c r="AF62" s="0">
-        <v>44.36</v>
+        <v>44.63</v>
       </c>
       <c r="AG62" s="0">
-        <v>34.7</v>
+        <v>34.69</v>
       </c>
       <c r="AH62" s="0">
-        <v>34.7</v>
+        <v>34.69</v>
       </c>
       <c r="AI62" s="0" t="s">
         <v>47</v>
@@ -7517,52 +7502,52 @@
         <v>46</v>
       </c>
       <c r="N63" s="0">
-        <v>340.68</v>
+        <v>330.975</v>
       </c>
       <c r="O63" s="0">
-        <v>89.8</v>
+        <v>89.56</v>
       </c>
       <c r="P63" s="0">
         <v>0</v>
       </c>
       <c r="Q63" s="0">
-        <v>1.18981</v>
+        <v>1.11169</v>
       </c>
       <c r="R63" s="0">
-        <v>1.1447</v>
+        <v>1.11596</v>
       </c>
       <c r="S63" s="0">
         <v>0</v>
       </c>
       <c r="T63" s="0">
+        <v>316</v>
+      </c>
+      <c r="U63" s="0">
+        <v>130</v>
+      </c>
+      <c r="V63" s="0">
         <v>313</v>
       </c>
-      <c r="U63" s="0">
-        <v>127</v>
-      </c>
-      <c r="V63" s="0">
-        <v>311</v>
-      </c>
       <c r="W63" s="0">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="X63" s="0">
-        <v>6.78</v>
+        <v>6.81</v>
       </c>
       <c r="Y63" s="0">
-        <v>7.47</v>
+        <v>7.52</v>
       </c>
       <c r="Z63" s="0">
-        <v>7.47</v>
+        <v>7.52</v>
       </c>
       <c r="AA63" s="0">
-        <v>-6.653</v>
+        <v>-6.902</v>
       </c>
       <c r="AB63" s="0">
-        <v>-9.284</v>
+        <v>-9.639</v>
       </c>
       <c r="AC63" s="0">
-        <v>4.73</v>
+        <v>4.72</v>
       </c>
       <c r="AD63" s="0">
         <v>5.22</v>
@@ -7571,7 +7556,7 @@
         <v>5.22</v>
       </c>
       <c r="AF63" s="0">
-        <v>0.16</v>
+        <v>0.15</v>
       </c>
       <c r="AG63" s="0">
         <v>0.34</v>
@@ -7624,67 +7609,67 @@
         <v>97</v>
       </c>
       <c r="N64" s="0">
-        <v>340.68</v>
+        <v>330.975</v>
       </c>
       <c r="O64" s="0">
-        <v>32.04</v>
+        <v>53.6</v>
       </c>
       <c r="P64" s="0">
         <v>0</v>
       </c>
       <c r="Q64" s="0">
-        <v>0.42451</v>
+        <v>0.66533</v>
       </c>
       <c r="R64" s="0">
-        <v>1.00905</v>
+        <v>0.98371</v>
       </c>
       <c r="S64" s="0">
         <v>0</v>
       </c>
       <c r="T64" s="0">
-        <v>1394</v>
+        <v>740</v>
       </c>
       <c r="U64" s="0">
-        <v>1055</v>
+        <v>401</v>
       </c>
       <c r="V64" s="0">
-        <v>563</v>
+        <v>478</v>
       </c>
       <c r="W64" s="0">
-        <v>210</v>
+        <v>125</v>
       </c>
       <c r="X64" s="0">
-        <v>18.31</v>
+        <v>11.64</v>
       </c>
       <c r="Y64" s="0">
-        <v>44.62</v>
+        <v>25.08</v>
       </c>
       <c r="Z64" s="0">
-        <v>44.62</v>
+        <v>25.08</v>
       </c>
       <c r="AA64" s="0">
-        <v>-62.217</v>
+        <v>-35.54</v>
       </c>
       <c r="AB64" s="0">
-        <v>-63.857</v>
+        <v>-36.78</v>
       </c>
       <c r="AC64" s="0">
-        <v>-3.29</v>
+        <v>-1.33</v>
       </c>
       <c r="AD64" s="0">
-        <v>2.47</v>
+        <v>2.8</v>
       </c>
       <c r="AE64" s="0">
-        <v>2.47</v>
+        <v>2.8</v>
       </c>
       <c r="AF64" s="0">
-        <v>-0.97</v>
+        <v>-0.9</v>
       </c>
       <c r="AG64" s="0">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="AH64" s="0">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="AI64" s="0" t="s">
         <v>47</v>
@@ -7731,61 +7716,61 @@
         <v>270</v>
       </c>
       <c r="N65" s="0">
-        <v>613.565</v>
+        <v>596.086</v>
       </c>
       <c r="O65" s="0">
-        <v>109.32</v>
+        <v>106.32</v>
       </c>
       <c r="P65" s="0">
         <v>0</v>
       </c>
       <c r="Q65" s="0">
-        <v>2.60864</v>
+        <v>2.37683</v>
       </c>
       <c r="R65" s="0">
-        <v>2.37191</v>
+        <v>2.31236</v>
       </c>
       <c r="S65" s="0">
         <v>0</v>
       </c>
       <c r="T65" s="0">
-        <v>310</v>
+        <v>325</v>
       </c>
       <c r="U65" s="0">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="V65" s="0">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="W65" s="0">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="X65" s="0">
-        <v>6.59</v>
+        <v>6.88</v>
       </c>
       <c r="Y65" s="0">
-        <v>6.17</v>
+        <v>7.6</v>
       </c>
       <c r="Z65" s="0">
-        <v>6.17</v>
+        <v>7.6</v>
       </c>
       <c r="AA65" s="0">
-        <v>-1.229</v>
+        <v>-1.539</v>
       </c>
       <c r="AB65" s="0">
-        <v>-2.691</v>
+        <v>-3.041</v>
       </c>
       <c r="AC65" s="0">
-        <v>1.86</v>
+        <v>1.91</v>
       </c>
       <c r="AD65" s="0">
-        <v>1.98</v>
+        <v>1.96</v>
       </c>
       <c r="AE65" s="0">
-        <v>1.98</v>
+        <v>1.96</v>
       </c>
       <c r="AF65" s="0">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="AG65" s="0">
         <v>0.06</v>

</xml_diff>